<commit_message>
Fix classification of Ghai samples in metadata file
</commit_message>
<xml_diff>
--- a/metadata/2015-07-13 actinos Metadata (formatted).xlsx
+++ b/metadata/2015-07-13 actinos Metadata (formatted).xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="1560" windowWidth="22580" windowHeight="13980" tabRatio="500"/>
+    <workbookView xWindow="-29280" yWindow="-4920" windowWidth="22580" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="244">
   <si>
     <t>Composite genome from Lake Mendota Epilimnion pan-assembly MEint.metabat.6647</t>
   </si>
@@ -1396,9 +1396,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1407,6 +1404,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="514">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2278,7 +2278,7 @@
     <col min="23" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="21" customFormat="1" ht="36">
+    <row r="1" spans="1:22" s="20" customFormat="1" ht="36">
       <c r="A1" s="11" t="s">
         <v>67</v>
       </c>
@@ -7032,63 +7032,74 @@
       <c r="A68" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="B68" s="13"/>
+      <c r="B68" s="14" t="s">
+        <v>171</v>
+      </c>
       <c r="C68" s="13"/>
-      <c r="D68" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
+      <c r="D68" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>227</v>
+      </c>
       <c r="G68" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="H68" s="13">
-        <v>973536</v>
-      </c>
-      <c r="I68" s="18">
-        <v>0.97</v>
-      </c>
-      <c r="J68" s="18">
-        <v>0.97</v>
-      </c>
-      <c r="K68" s="13">
-        <v>37</v>
-      </c>
-      <c r="L68" s="13">
-        <v>37</v>
-      </c>
-      <c r="M68" s="13">
-        <v>965</v>
+        <v>230</v>
+      </c>
+      <c r="H68" s="14">
+        <v>2690660</v>
+      </c>
+      <c r="I68" s="15">
+        <f>H68/1000000</f>
+        <v>2.6906599999999998</v>
+      </c>
+      <c r="J68" s="15">
+        <f>I68</f>
+        <v>2.6906599999999998</v>
+      </c>
+      <c r="K68" s="14">
+        <v>132</v>
+      </c>
+      <c r="L68" s="14">
+        <f>K68</f>
+        <v>132</v>
+      </c>
+      <c r="M68" s="14">
+        <v>2884</v>
       </c>
       <c r="N68" s="14">
-        <f t="shared" ref="N68:N69" si="17">M68</f>
-        <v>965</v>
-      </c>
-      <c r="O68" s="18">
-        <v>0.56999999999999995</v>
+        <f>M68</f>
+        <v>2884</v>
+      </c>
+      <c r="O68" s="15">
+        <v>0.52149999999999996</v>
       </c>
       <c r="P68" s="14">
-        <f t="shared" ref="P68:P69" si="18">O68</f>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="Q68" s="13">
-        <v>29</v>
-      </c>
-      <c r="R68" s="18">
-        <v>0.78</v>
+        <f>O68</f>
+        <v>0.52149999999999996</v>
+      </c>
+      <c r="Q68" s="14">
+        <v>34</v>
+      </c>
+      <c r="R68" s="15">
+        <f>Q68/37</f>
+        <v>0.91891891891891897</v>
       </c>
       <c r="S68" s="15">
-        <f t="shared" ref="S68:S78" si="19">R68</f>
-        <v>0.78</v>
-      </c>
-      <c r="T68" s="18">
-        <v>1.24</v>
+        <f>R68</f>
+        <v>0.91891891891891897</v>
+      </c>
+      <c r="T68" s="15">
+        <f>I68/R68</f>
+        <v>2.928071176470588</v>
       </c>
       <c r="U68" s="15">
-        <f t="shared" ref="U68:U69" si="20">T68</f>
-        <v>1.24</v>
-      </c>
-      <c r="V68" s="19">
+        <f>T68</f>
+        <v>2.928071176470588</v>
+      </c>
+      <c r="V68" s="16">
         <v>4</v>
       </c>
     </row>
@@ -7096,63 +7107,71 @@
       <c r="A69" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="B69" s="13"/>
+      <c r="B69" s="13" t="s">
+        <v>169</v>
+      </c>
       <c r="C69" s="13"/>
       <c r="D69" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
+      <c r="E69" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>227</v>
+      </c>
       <c r="G69" s="13" t="s">
         <v>231</v>
       </c>
       <c r="H69" s="13">
-        <v>1242025</v>
-      </c>
-      <c r="I69" s="18">
+        <v>973536</v>
+      </c>
+      <c r="I69" s="17">
+        <v>0.97</v>
+      </c>
+      <c r="J69" s="15">
+        <f t="shared" ref="J69:J78" si="17">I69</f>
+        <v>0.97</v>
+      </c>
+      <c r="K69" s="13">
+        <v>37</v>
+      </c>
+      <c r="L69" s="14">
+        <f t="shared" ref="L69:L78" si="18">K69</f>
+        <v>37</v>
+      </c>
+      <c r="M69" s="13">
+        <v>965</v>
+      </c>
+      <c r="N69" s="14">
+        <f t="shared" ref="N69:N78" si="19">M69</f>
+        <v>965</v>
+      </c>
+      <c r="O69" s="17">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="P69" s="14">
+        <f t="shared" ref="P69:P78" si="20">O69</f>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q69" s="13">
+        <v>29</v>
+      </c>
+      <c r="R69" s="17">
+        <v>0.78</v>
+      </c>
+      <c r="S69" s="15">
+        <f>R69</f>
+        <v>0.78</v>
+      </c>
+      <c r="T69" s="17">
         <v>1.24</v>
       </c>
-      <c r="J69" s="18">
+      <c r="U69" s="15">
+        <f t="shared" ref="U69:U78" si="21">T69</f>
         <v>1.24</v>
       </c>
-      <c r="K69" s="13">
-        <v>10</v>
-      </c>
-      <c r="L69" s="13">
-        <v>10</v>
-      </c>
-      <c r="M69" s="13">
-        <v>1259</v>
-      </c>
-      <c r="N69" s="14">
-        <f t="shared" si="17"/>
-        <v>1259</v>
-      </c>
-      <c r="O69" s="18">
-        <v>0.44</v>
-      </c>
-      <c r="P69" s="14">
-        <f t="shared" si="18"/>
-        <v>0.44</v>
-      </c>
-      <c r="Q69" s="13">
-        <v>36</v>
-      </c>
-      <c r="R69" s="18">
-        <v>0.97</v>
-      </c>
-      <c r="S69" s="15">
-        <f t="shared" si="19"/>
-        <v>0.97</v>
-      </c>
-      <c r="T69" s="18">
-        <v>1.28</v>
-      </c>
-      <c r="U69" s="15">
-        <f t="shared" si="20"/>
-        <v>1.28</v>
-      </c>
-      <c r="V69" s="19">
+      <c r="V69" s="18">
         <v>4</v>
       </c>
     </row>
@@ -7160,10 +7179,12 @@
       <c r="A70" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="B70" s="14"/>
+      <c r="B70" s="13" t="s">
+        <v>170</v>
+      </c>
       <c r="C70" s="14"/>
-      <c r="D70" s="14" t="s">
-        <v>119</v>
+      <c r="D70" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="E70" s="13" t="s">
         <v>227</v>
@@ -7172,60 +7193,57 @@
         <v>227</v>
       </c>
       <c r="G70" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="H70" s="14">
-        <v>2690660</v>
-      </c>
-      <c r="I70" s="15">
-        <f t="shared" ref="I70:I78" si="21">H70/1000000</f>
-        <v>2.6906599999999998</v>
+        <v>231</v>
+      </c>
+      <c r="H70" s="13">
+        <v>1242025</v>
+      </c>
+      <c r="I70" s="17">
+        <v>1.24</v>
       </c>
       <c r="J70" s="15">
-        <f t="shared" ref="J70:J78" si="22">I70</f>
-        <v>2.6906599999999998</v>
-      </c>
-      <c r="K70" s="14">
-        <v>132</v>
+        <f t="shared" si="17"/>
+        <v>1.24</v>
+      </c>
+      <c r="K70" s="13">
+        <v>10</v>
       </c>
       <c r="L70" s="14">
-        <f t="shared" ref="L70:L78" si="23">K70</f>
-        <v>132</v>
-      </c>
-      <c r="M70" s="14">
-        <v>2884</v>
+        <f t="shared" si="18"/>
+        <v>10</v>
+      </c>
+      <c r="M70" s="13">
+        <v>1259</v>
       </c>
       <c r="N70" s="14">
-        <f t="shared" ref="N70:N78" si="24">M70</f>
-        <v>2884</v>
-      </c>
-      <c r="O70" s="15">
-        <v>0.52149999999999996</v>
+        <f t="shared" si="19"/>
+        <v>1259</v>
+      </c>
+      <c r="O70" s="17">
+        <v>0.44</v>
       </c>
       <c r="P70" s="14">
-        <f t="shared" ref="P70:P78" si="25">O70</f>
-        <v>0.52149999999999996</v>
-      </c>
-      <c r="Q70" s="14">
-        <v>34</v>
-      </c>
-      <c r="R70" s="15">
-        <f t="shared" ref="R70:R78" si="26">Q70/37</f>
-        <v>0.91891891891891897</v>
+        <f t="shared" si="20"/>
+        <v>0.44</v>
+      </c>
+      <c r="Q70" s="13">
+        <v>36</v>
+      </c>
+      <c r="R70" s="17">
+        <v>0.97</v>
       </c>
       <c r="S70" s="15">
-        <f t="shared" si="19"/>
-        <v>0.91891891891891897</v>
-      </c>
-      <c r="T70" s="15">
-        <f t="shared" ref="T70:T78" si="27">I70/R70</f>
-        <v>2.928071176470588</v>
+        <f>R70</f>
+        <v>0.97</v>
+      </c>
+      <c r="T70" s="17">
+        <v>1.28</v>
       </c>
       <c r="U70" s="15">
-        <f t="shared" ref="U70:U78" si="28">T70</f>
-        <v>2.928071176470588</v>
-      </c>
-      <c r="V70" s="16">
+        <f t="shared" si="21"/>
+        <v>1.28</v>
+      </c>
+      <c r="V70" s="18">
         <v>4</v>
       </c>
     </row>
@@ -7233,7 +7251,9 @@
       <c r="A71" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="B71" s="14"/>
+      <c r="B71" s="14" t="s">
+        <v>172</v>
+      </c>
       <c r="C71" s="14"/>
       <c r="D71" s="13" t="s">
         <v>103</v>
@@ -7251,51 +7271,51 @@
         <v>523140</v>
       </c>
       <c r="I71" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="I71:I78" si="22">H71/1000000</f>
         <v>0.52314000000000005</v>
       </c>
       <c r="J71" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>0.52314000000000005</v>
       </c>
       <c r="K71" s="14">
         <v>31</v>
       </c>
       <c r="L71" s="14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>31</v>
       </c>
       <c r="M71" s="14">
         <v>551</v>
       </c>
       <c r="N71" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>551</v>
       </c>
       <c r="O71" s="15">
         <v>0.42059999999999997</v>
       </c>
       <c r="P71" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>0.42059999999999997</v>
       </c>
       <c r="Q71" s="14">
         <v>3</v>
       </c>
       <c r="R71" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="R71:R78" si="23">Q71/37</f>
         <v>8.1081081081081086E-2</v>
       </c>
       <c r="S71" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="S71:S78" si="24">R71</f>
         <v>8.1081081081081086E-2</v>
       </c>
       <c r="T71" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="T71:T78" si="25">I71/R71</f>
         <v>6.4520600000000004</v>
       </c>
       <c r="U71" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>6.4520600000000004</v>
       </c>
       <c r="V71" s="16">
@@ -7306,7 +7326,9 @@
       <c r="A72" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="B72" s="14"/>
+      <c r="B72" s="14" t="s">
+        <v>173</v>
+      </c>
       <c r="C72" s="14"/>
       <c r="D72" s="13" t="s">
         <v>103</v>
@@ -7324,51 +7346,51 @@
         <v>974886</v>
       </c>
       <c r="I72" s="15">
-        <f t="shared" si="21"/>
-        <v>0.97488600000000003</v>
-      </c>
-      <c r="J72" s="15">
         <f t="shared" si="22"/>
         <v>0.97488600000000003</v>
       </c>
+      <c r="J72" s="15">
+        <f t="shared" si="17"/>
+        <v>0.97488600000000003</v>
+      </c>
       <c r="K72" s="14">
         <v>66</v>
       </c>
       <c r="L72" s="14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>66</v>
       </c>
       <c r="M72" s="14">
         <v>1004</v>
       </c>
       <c r="N72" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>1004</v>
       </c>
       <c r="O72" s="15">
         <v>0.4042</v>
       </c>
       <c r="P72" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>0.4042</v>
       </c>
       <c r="Q72" s="14">
         <v>6</v>
       </c>
       <c r="R72" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>0.16216216216216217</v>
       </c>
       <c r="S72" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.16216216216216217</v>
       </c>
       <c r="T72" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>6.0117969999999996</v>
       </c>
       <c r="U72" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>6.0117969999999996</v>
       </c>
       <c r="V72" s="16">
@@ -7379,7 +7401,9 @@
       <c r="A73" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B73" s="14"/>
+      <c r="B73" s="14" t="s">
+        <v>167</v>
+      </c>
       <c r="C73" s="14"/>
       <c r="D73" s="14" t="s">
         <v>232</v>
@@ -7397,51 +7421,51 @@
         <v>856463</v>
       </c>
       <c r="I73" s="15">
-        <f t="shared" si="21"/>
-        <v>0.85646299999999997</v>
-      </c>
-      <c r="J73" s="15">
         <f t="shared" si="22"/>
         <v>0.85646299999999997</v>
       </c>
+      <c r="J73" s="15">
+        <f t="shared" si="17"/>
+        <v>0.85646299999999997</v>
+      </c>
       <c r="K73" s="14">
         <v>36</v>
       </c>
       <c r="L73" s="14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>36</v>
       </c>
       <c r="M73" s="14">
         <v>873</v>
       </c>
       <c r="N73" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>873</v>
       </c>
       <c r="O73" s="15">
         <v>0.61639999999999995</v>
       </c>
       <c r="P73" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>0.61639999999999995</v>
       </c>
       <c r="Q73" s="14">
         <v>29</v>
       </c>
       <c r="R73" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>0.78378378378378377</v>
       </c>
       <c r="S73" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.78378378378378377</v>
       </c>
       <c r="T73" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>1.0927286551724138</v>
       </c>
       <c r="U73" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>1.0927286551724138</v>
       </c>
       <c r="V73" s="16">
@@ -7452,7 +7476,9 @@
       <c r="A74" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B74" s="14"/>
+      <c r="B74" s="14" t="s">
+        <v>168</v>
+      </c>
       <c r="C74" s="14"/>
       <c r="D74" s="14" t="s">
         <v>232</v>
@@ -7470,51 +7496,51 @@
         <v>1083653</v>
       </c>
       <c r="I74" s="15">
-        <f t="shared" si="21"/>
-        <v>1.083653</v>
-      </c>
-      <c r="J74" s="15">
         <f t="shared" si="22"/>
         <v>1.083653</v>
       </c>
+      <c r="J74" s="15">
+        <f t="shared" si="17"/>
+        <v>1.083653</v>
+      </c>
       <c r="K74" s="14">
         <v>15</v>
       </c>
       <c r="L74" s="14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="M74" s="14">
         <v>1114</v>
       </c>
       <c r="N74" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>1114</v>
       </c>
       <c r="O74" s="15">
         <v>0.59279999999999999</v>
       </c>
       <c r="P74" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>0.59279999999999999</v>
       </c>
       <c r="Q74" s="14">
         <v>33</v>
       </c>
       <c r="R74" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>0.89189189189189189</v>
       </c>
       <c r="S74" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.89189189189189189</v>
       </c>
       <c r="T74" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>1.2150048787878787</v>
       </c>
       <c r="U74" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>1.2150048787878787</v>
       </c>
       <c r="V74" s="16">
@@ -7525,7 +7551,9 @@
       <c r="A75" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="B75" s="14"/>
+      <c r="B75" s="14" t="s">
+        <v>174</v>
+      </c>
       <c r="C75" s="14"/>
       <c r="D75" s="14" t="s">
         <v>103</v>
@@ -7543,49 +7571,49 @@
         <v>979038</v>
       </c>
       <c r="I75" s="15">
-        <f t="shared" si="21"/>
-        <v>0.97903799999999996</v>
-      </c>
-      <c r="J75" s="15">
         <f t="shared" si="22"/>
         <v>0.97903799999999996</v>
       </c>
+      <c r="J75" s="15">
+        <f t="shared" si="17"/>
+        <v>0.97903799999999996</v>
+      </c>
       <c r="K75" s="14">
         <v>95</v>
       </c>
       <c r="L75" s="14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>95</v>
       </c>
       <c r="M75" s="14">
         <v>1171</v>
       </c>
       <c r="N75" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>1171</v>
       </c>
       <c r="O75" s="14"/>
       <c r="P75" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Q75" s="14">
         <v>24</v>
       </c>
       <c r="R75" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>0.64864864864864868</v>
       </c>
       <c r="S75" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.64864864864864868</v>
       </c>
       <c r="T75" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>1.5093502499999998</v>
       </c>
       <c r="U75" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>1.5093502499999998</v>
       </c>
       <c r="V75" s="16">
@@ -7596,7 +7624,9 @@
       <c r="A76" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="B76" s="14"/>
+      <c r="B76" s="14" t="s">
+        <v>175</v>
+      </c>
       <c r="C76" s="14"/>
       <c r="D76" s="14" t="s">
         <v>119</v>
@@ -7614,49 +7644,49 @@
         <v>1340901</v>
       </c>
       <c r="I76" s="15">
-        <f t="shared" si="21"/>
-        <v>1.3409009999999999</v>
-      </c>
-      <c r="J76" s="15">
         <f t="shared" si="22"/>
         <v>1.3409009999999999</v>
       </c>
+      <c r="J76" s="15">
+        <f t="shared" si="17"/>
+        <v>1.3409009999999999</v>
+      </c>
       <c r="K76" s="14">
         <v>384</v>
       </c>
       <c r="L76" s="14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>384</v>
       </c>
       <c r="M76" s="14">
         <v>1849</v>
       </c>
       <c r="N76" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>1849</v>
       </c>
       <c r="O76" s="14"/>
       <c r="P76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Q76" s="14">
         <v>23</v>
       </c>
       <c r="R76" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>0.6216216216216216</v>
       </c>
       <c r="S76" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.6216216216216216</v>
       </c>
       <c r="T76" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>2.157101608695652</v>
       </c>
       <c r="U76" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>2.157101608695652</v>
       </c>
       <c r="V76" s="16">
@@ -7664,11 +7694,15 @@
       </c>
     </row>
     <row r="77" spans="1:22">
-      <c r="A77" s="20" t="s">
+      <c r="A77" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="B77" s="20"/>
-      <c r="C77" s="20"/>
+      <c r="B77" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C77" s="14">
+        <v>2596583567</v>
+      </c>
       <c r="D77" s="14" t="s">
         <v>179</v>
       </c>
@@ -7685,63 +7719,67 @@
         <v>2582396</v>
       </c>
       <c r="I77" s="15">
+        <f t="shared" si="22"/>
+        <v>2.5823960000000001</v>
+      </c>
+      <c r="J77" s="15">
+        <f t="shared" si="17"/>
+        <v>2.5823960000000001</v>
+      </c>
+      <c r="K77" s="14">
+        <v>13</v>
+      </c>
+      <c r="L77" s="14">
+        <f t="shared" si="18"/>
+        <v>13</v>
+      </c>
+      <c r="M77" s="14">
+        <v>2415</v>
+      </c>
+      <c r="N77" s="14">
+        <f t="shared" si="19"/>
+        <v>2415</v>
+      </c>
+      <c r="O77" s="14">
+        <v>0.61</v>
+      </c>
+      <c r="P77" s="14">
+        <f t="shared" si="20"/>
+        <v>0.61</v>
+      </c>
+      <c r="Q77" s="14">
+        <v>37</v>
+      </c>
+      <c r="R77" s="15">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="S77" s="15">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="T77" s="15">
+        <f t="shared" si="25"/>
+        <v>2.5823960000000001</v>
+      </c>
+      <c r="U77" s="15">
         <f t="shared" si="21"/>
         <v>2.5823960000000001</v>
       </c>
-      <c r="J77" s="15">
-        <f t="shared" si="22"/>
-        <v>2.5823960000000001</v>
-      </c>
-      <c r="K77" s="14">
-        <v>385</v>
-      </c>
-      <c r="L77" s="14">
-        <f t="shared" si="23"/>
-        <v>385</v>
-      </c>
-      <c r="M77" s="14">
-        <v>2415</v>
-      </c>
-      <c r="N77" s="14">
-        <f t="shared" si="24"/>
-        <v>2415</v>
-      </c>
-      <c r="O77" s="14">
-        <v>0.61</v>
-      </c>
-      <c r="P77" s="14">
-        <f t="shared" si="25"/>
-        <v>0.61</v>
-      </c>
-      <c r="Q77" s="14">
-        <v>37</v>
-      </c>
-      <c r="R77" s="15">
-        <f t="shared" si="26"/>
-        <v>1</v>
-      </c>
-      <c r="S77" s="15">
-        <f t="shared" si="19"/>
-        <v>1</v>
-      </c>
-      <c r="T77" s="15">
-        <f t="shared" si="27"/>
-        <v>2.5823960000000001</v>
-      </c>
-      <c r="U77" s="15">
-        <f t="shared" si="28"/>
-        <v>2.5823960000000001</v>
-      </c>
       <c r="V77" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:22">
-      <c r="A78" s="20" t="s">
+      <c r="A78" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="B78" s="20"/>
-      <c r="C78" s="20"/>
+      <c r="B78" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C78" s="14">
+        <v>2596583568</v>
+      </c>
       <c r="D78" s="14" t="s">
         <v>103</v>
       </c>
@@ -7758,52 +7796,52 @@
         <v>1964596</v>
       </c>
       <c r="I78" s="15">
-        <f t="shared" si="21"/>
-        <v>1.964596</v>
-      </c>
-      <c r="J78" s="15">
         <f t="shared" si="22"/>
         <v>1.964596</v>
       </c>
+      <c r="J78" s="15">
+        <f t="shared" si="17"/>
+        <v>1.964596</v>
+      </c>
       <c r="K78" s="14">
-        <v>386</v>
+        <v>105</v>
       </c>
       <c r="L78" s="14">
-        <f t="shared" si="23"/>
-        <v>386</v>
+        <f t="shared" si="18"/>
+        <v>105</v>
       </c>
       <c r="M78" s="14">
         <v>2108</v>
       </c>
       <c r="N78" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>2108</v>
       </c>
       <c r="O78" s="14">
         <v>0.49</v>
       </c>
       <c r="P78" s="14">
+        <f t="shared" si="20"/>
+        <v>0.49</v>
+      </c>
+      <c r="Q78" s="14">
+        <v>13</v>
+      </c>
+      <c r="R78" s="15">
+        <f t="shared" si="23"/>
+        <v>0.35135135135135137</v>
+      </c>
+      <c r="S78" s="15">
+        <f t="shared" si="24"/>
+        <v>0.35135135135135137</v>
+      </c>
+      <c r="T78" s="15">
         <f t="shared" si="25"/>
-        <v>0.49</v>
-      </c>
-      <c r="Q78" s="14">
-        <v>12</v>
-      </c>
-      <c r="R78" s="15">
-        <f t="shared" si="26"/>
-        <v>0.32432432432432434</v>
-      </c>
-      <c r="S78" s="15">
-        <f t="shared" si="19"/>
-        <v>0.32432432432432434</v>
-      </c>
-      <c r="T78" s="15">
-        <f t="shared" si="27"/>
-        <v>6.0575043333333332</v>
+        <v>5.5915424615384612</v>
       </c>
       <c r="U78" s="15">
-        <f t="shared" si="28"/>
-        <v>6.0575043333333332</v>
+        <f t="shared" si="21"/>
+        <v>5.5915424615384612</v>
       </c>
       <c r="V78" s="16">
         <v>2</v>
@@ -7813,8 +7851,8 @@
   <sortState ref="A2:U60">
     <sortCondition ref="A71"/>
   </sortState>
-  <conditionalFormatting sqref="P59:P60 P2:P47 P63:P78">
-    <cfRule type="dataBar" priority="8">
+  <conditionalFormatting sqref="P59:P60 P2:P47 P63:P67">
+    <cfRule type="dataBar" priority="14">
       <dataBar showValue="0">
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7827,8 +7865,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J70:J78 J63:J67 J59:J60 J2:J47">
-    <cfRule type="dataBar" priority="9">
+  <conditionalFormatting sqref="J63:J67 J59:J60 J2:J47">
+    <cfRule type="dataBar" priority="15">
       <dataBar showValue="0">
         <cfvo type="num" val="0"/>
         <cfvo type="max"/>
@@ -7841,8 +7879,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L70:L78 L63:L67 L2:L47 L59:L60">
-    <cfRule type="dataBar" priority="10">
+  <conditionalFormatting sqref="L63:L67 L2:L47 L59:L60">
+    <cfRule type="dataBar" priority="16">
       <dataBar showValue="0">
         <cfvo type="num" val="0"/>
         <cfvo type="max"/>
@@ -7855,8 +7893,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N47 N59:N60 N63:N78">
-    <cfRule type="dataBar" priority="11">
+  <conditionalFormatting sqref="N2:N47 N59:N60 N63:N67">
+    <cfRule type="dataBar" priority="17">
       <dataBar showValue="0">
         <cfvo type="num" val="0"/>
         <cfvo type="max"/>
@@ -7870,7 +7908,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:J56">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="13">
       <dataBar showValue="0">
         <cfvo type="num" val="0"/>
         <cfvo type="max"/>
@@ -7884,7 +7922,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L48:L56">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="12">
       <dataBar showValue="0">
         <cfvo type="num" val="0"/>
         <cfvo type="max"/>
@@ -7898,7 +7936,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48:N56">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="11">
       <dataBar showValue="0">
         <cfvo type="num" val="0"/>
         <cfvo type="max"/>
@@ -7912,7 +7950,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P48:P56">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="10">
       <dataBar showValue="0">
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7925,8 +7963,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U78">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="U2:U67">
+    <cfRule type="dataBar" priority="8">
       <dataBar showValue="0">
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7939,7 +7977,35 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S78">
+  <conditionalFormatting sqref="S2:S67">
+    <cfRule type="dataBar" priority="7">
+      <dataBar showValue="0">
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="8"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{13A4F9F9-CECB-014E-B329-FE54C18B9928}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P68:P78">
+    <cfRule type="dataBar" priority="2">
+      <dataBar showValue="0">
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="7"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0ACB48A8-A164-4B40-A584-3EA0D93DC271}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S68:S78">
     <cfRule type="dataBar" priority="1">
       <dataBar showValue="0">
         <cfvo type="num" val="0"/>
@@ -7948,7 +8014,63 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{13A4F9F9-CECB-014E-B329-FE54C18B9928}</x14:id>
+          <x14:id>{6C27E804-1EA1-5742-9B91-AD94F1C6E924}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N68:N78">
+    <cfRule type="dataBar" priority="3">
+      <dataBar showValue="0">
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color theme="6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{54F64201-BEA4-C347-ADEC-6B497D33FCAD}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U68:U78">
+    <cfRule type="dataBar" priority="4">
+      <dataBar showValue="0">
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AC7949A4-8D07-3844-AFC3-2F5FF32B05E1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J68:J78">
+    <cfRule type="dataBar" priority="5">
+      <dataBar showValue="0">
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color theme="5"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{19CF9985-B805-3540-B9BA-10A7FFACEA59}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L68:L78">
+    <cfRule type="dataBar" priority="6">
+      <dataBar showValue="0">
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color theme="4"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{56AA5627-8FF5-314F-AF70-3D60FE7ED167}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -7972,7 +8094,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>P59:P60 P2:P47 P63:P78</xm:sqref>
+          <xm:sqref>P59:P60 P2:P47 P63:P67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{939C3852-ED43-CE40-8F41-2DC027965E28}">
@@ -7985,7 +8107,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J70:J78 J63:J67 J59:J60 J2:J47</xm:sqref>
+          <xm:sqref>J63:J67 J59:J60 J2:J47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{833D25C6-74DA-5D42-B771-B46958310B4A}">
@@ -7998,7 +8120,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L70:L78 L63:L67 L2:L47 L59:L60</xm:sqref>
+          <xm:sqref>L63:L67 L2:L47 L59:L60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{64C0CA63-77D7-514F-9163-3243A9B4177A}">
@@ -8011,7 +8133,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>N2:N47 N59:N60 N63:N78</xm:sqref>
+          <xm:sqref>N2:N47 N59:N60 N63:N67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5FD8FAA8-BFBB-314C-91CD-712E409B4A9D}">
@@ -8078,7 +8200,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U2:U78</xm:sqref>
+          <xm:sqref>U2:U67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{13A4F9F9-CECB-014E-B329-FE54C18B9928}">
@@ -8094,7 +8216,90 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>S2:S78</xm:sqref>
+          <xm:sqref>S2:S67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0ACB48A8-A164-4B40-A584-3EA0D93DC271}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:borderColor rgb="FF000000"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P68:P78</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6C27E804-1EA1-5742-9B91-AD94F1C6E924}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:borderColor rgb="FF000000"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>S68:S78</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{54F64201-BEA4-C347-ADEC-6B497D33FCAD}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarColorSameAsPositive="1">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="max"/>
+              <x14:borderColor rgb="FF000000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N68:N78</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AC7949A4-8D07-3844-AFC3-2F5FF32B05E1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="max"/>
+              <x14:borderColor rgb="FF000000"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>U68:U78</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{19CF9985-B805-3540-B9BA-10A7FFACEA59}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarColorSameAsPositive="1">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="max"/>
+              <x14:borderColor rgb="FF000000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J68:J78</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{56AA5627-8FF5-314F-AF70-3D60FE7ED167}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarColorSameAsPositive="1">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="max"/>
+              <x14:borderColor rgb="FF000000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L68:L78</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -10101,14 +10306,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="17"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
Update metadata for newly classifed samples.
Recolor phylogenetic tree. Update taxonomy.csv and metadata.xls taxonomy files.
</commit_message>
<xml_diff>
--- a/metadata/2015-07-13 actinos Metadata (formatted).xlsx
+++ b/metadata/2015-07-13 actinos Metadata (formatted).xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="245">
   <si>
     <t>Composite genome from Lake Mendota Epilimnion pan-assembly MEint.metabat.6647</t>
   </si>
@@ -759,6 +759,9 @@
   </si>
   <si>
     <t>AP actinobacterium SCGC AAA028-K151372485236459</t>
+  </si>
+  <si>
+    <t>ANI and Coverage</t>
   </si>
 </sst>
 </file>
@@ -838,7 +841,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="514">
+  <cellStyleXfs count="520">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1350,6 +1353,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1408,7 +1417,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="514">
+  <cellStyles count="520">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1668,6 +1677,9 @@
     <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="511" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="513" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="515" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="517" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="519" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1922,6 +1934,9 @@
     <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="512" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="514" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="516" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="518" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2254,8 +2269,8 @@
   <dimension ref="A1:V78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -3902,11 +3917,11 @@
       <c r="E22" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>225</v>
+      <c r="F22" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>244</v>
       </c>
       <c r="H22" s="14">
         <v>1144269</v>
@@ -5285,14 +5300,14 @@
       <c r="D40" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E40" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>227</v>
+      <c r="E40" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>123</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="H40" s="14">
         <v>1793743</v>

</xml_diff>

<commit_message>
Fix error in metadata re: Meint4252 GFM
</commit_message>
<xml_diff>
--- a/metadata/2015-07-13 actinos Metadata (formatted).xlsx
+++ b/metadata/2015-07-13 actinos Metadata (formatted).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-29280" yWindow="-4920" windowWidth="22580" windowHeight="13980" tabRatio="500"/>
+    <workbookView xWindow="-33280" yWindow="-4560" windowWidth="27940" windowHeight="16800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -2269,8 +2269,8 @@
   <dimension ref="A1:V78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -2387,39 +2387,39 @@
         <v>822296</v>
       </c>
       <c r="I2" s="15">
-        <f t="shared" ref="I2:I33" si="0">H2/1000000</f>
+        <f>H2/1000000</f>
         <v>0.82229600000000003</v>
       </c>
       <c r="J2" s="15">
-        <f t="shared" ref="J2:J33" si="1">I2</f>
+        <f>I2</f>
         <v>0.82229600000000003</v>
       </c>
       <c r="K2" s="14">
         <v>22</v>
       </c>
       <c r="L2" s="14">
-        <f t="shared" ref="L2:L33" si="2">K2</f>
+        <f>K2</f>
         <v>22</v>
       </c>
       <c r="M2" s="14">
         <v>863</v>
       </c>
       <c r="N2" s="14">
-        <f t="shared" ref="N2:N33" si="3">M2</f>
+        <f>M2</f>
         <v>863</v>
       </c>
       <c r="O2" s="14">
         <v>0.47</v>
       </c>
       <c r="P2" s="14">
-        <f t="shared" ref="P2:P33" si="4">O2</f>
+        <f>O2</f>
         <v>0.47</v>
       </c>
       <c r="Q2" s="14">
         <v>2</v>
       </c>
       <c r="R2" s="15">
-        <f t="shared" ref="R2:R33" si="5">Q2/37</f>
+        <f>Q2/37</f>
         <v>5.4054054054054057E-2</v>
       </c>
       <c r="S2" s="15">
@@ -2427,11 +2427,11 @@
         <v>5.4054054054054057E-2</v>
       </c>
       <c r="T2" s="15">
-        <f t="shared" ref="T2:T33" si="6">I2/R2</f>
+        <f>I2/R2</f>
         <v>15.212475999999999</v>
       </c>
       <c r="U2" s="15">
-        <f t="shared" ref="U2:U33" si="7">T2</f>
+        <f>T2</f>
         <v>15.212475999999999</v>
       </c>
       <c r="V2" s="16">
@@ -2464,51 +2464,51 @@
         <v>1138490</v>
       </c>
       <c r="I3" s="15">
-        <f t="shared" si="0"/>
+        <f>H3/1000000</f>
         <v>1.13849</v>
       </c>
       <c r="J3" s="15">
-        <f t="shared" si="1"/>
+        <f>I3</f>
         <v>1.13849</v>
       </c>
       <c r="K3" s="14">
         <v>43</v>
       </c>
       <c r="L3" s="14">
-        <f t="shared" si="2"/>
+        <f>K3</f>
         <v>43</v>
       </c>
       <c r="M3" s="14">
         <v>1238</v>
       </c>
       <c r="N3" s="14">
-        <f t="shared" si="3"/>
+        <f>M3</f>
         <v>1238</v>
       </c>
       <c r="O3" s="14">
         <v>0.48</v>
       </c>
       <c r="P3" s="14">
-        <f t="shared" si="4"/>
+        <f>O3</f>
         <v>0.48</v>
       </c>
       <c r="Q3" s="14">
         <v>36</v>
       </c>
       <c r="R3" s="15">
-        <f t="shared" si="5"/>
+        <f>Q3/37</f>
         <v>0.97297297297297303</v>
       </c>
       <c r="S3" s="15">
-        <f t="shared" ref="S3:S65" si="8">R3</f>
+        <f>R3</f>
         <v>0.97297297297297303</v>
       </c>
       <c r="T3" s="15">
-        <f t="shared" si="6"/>
+        <f>I3/R3</f>
         <v>1.1701147222222221</v>
       </c>
       <c r="U3" s="15">
-        <f t="shared" si="7"/>
+        <f>T3</f>
         <v>1.1701147222222221</v>
       </c>
       <c r="V3" s="16">
@@ -2541,51 +2541,51 @@
         <v>1347568</v>
       </c>
       <c r="I4" s="15">
-        <f t="shared" si="0"/>
+        <f>H4/1000000</f>
         <v>1.3475680000000001</v>
       </c>
       <c r="J4" s="15">
-        <f t="shared" si="1"/>
+        <f>I4</f>
         <v>1.3475680000000001</v>
       </c>
       <c r="K4" s="14">
         <v>35</v>
       </c>
       <c r="L4" s="14">
-        <f t="shared" si="2"/>
+        <f>K4</f>
         <v>35</v>
       </c>
       <c r="M4" s="14">
         <v>1386</v>
       </c>
       <c r="N4" s="14">
-        <f t="shared" si="3"/>
+        <f>M4</f>
         <v>1386</v>
       </c>
       <c r="O4" s="14">
         <v>0.46</v>
       </c>
       <c r="P4" s="14">
-        <f t="shared" si="4"/>
+        <f>O4</f>
         <v>0.46</v>
       </c>
       <c r="Q4" s="14">
         <v>35</v>
       </c>
       <c r="R4" s="15">
-        <f t="shared" si="5"/>
+        <f>Q4/37</f>
         <v>0.94594594594594594</v>
       </c>
       <c r="S4" s="15">
-        <f t="shared" si="8"/>
+        <f>R4</f>
         <v>0.94594594594594594</v>
       </c>
       <c r="T4" s="15">
-        <f t="shared" si="6"/>
+        <f>I4/R4</f>
         <v>1.4245718857142857</v>
       </c>
       <c r="U4" s="15">
-        <f t="shared" si="7"/>
+        <f>T4</f>
         <v>1.4245718857142857</v>
       </c>
       <c r="V4" s="16">
@@ -2618,51 +2618,51 @@
         <v>1412935</v>
       </c>
       <c r="I5" s="15">
-        <f t="shared" si="0"/>
+        <f>H5/1000000</f>
         <v>1.4129350000000001</v>
       </c>
       <c r="J5" s="15">
-        <f t="shared" si="1"/>
+        <f>I5</f>
         <v>1.4129350000000001</v>
       </c>
       <c r="K5" s="14">
         <v>35</v>
       </c>
       <c r="L5" s="14">
-        <f t="shared" si="2"/>
+        <f>K5</f>
         <v>35</v>
       </c>
       <c r="M5" s="14">
         <v>1438</v>
       </c>
       <c r="N5" s="14">
-        <f t="shared" si="3"/>
+        <f>M5</f>
         <v>1438</v>
       </c>
       <c r="O5" s="14">
         <v>0.46</v>
       </c>
       <c r="P5" s="14">
-        <f t="shared" si="4"/>
+        <f>O5</f>
         <v>0.46</v>
       </c>
       <c r="Q5" s="14">
         <v>36</v>
       </c>
       <c r="R5" s="15">
-        <f t="shared" si="5"/>
+        <f>Q5/37</f>
         <v>0.97297297297297303</v>
       </c>
       <c r="S5" s="15">
-        <f t="shared" si="8"/>
+        <f>R5</f>
         <v>0.97297297297297303</v>
       </c>
       <c r="T5" s="15">
-        <f t="shared" si="6"/>
+        <f>I5/R5</f>
         <v>1.4521831944444443</v>
       </c>
       <c r="U5" s="15">
-        <f t="shared" si="7"/>
+        <f>T5</f>
         <v>1.4521831944444443</v>
       </c>
       <c r="V5" s="16">
@@ -2695,51 +2695,51 @@
         <v>884811</v>
       </c>
       <c r="I6" s="15">
-        <f t="shared" si="0"/>
+        <f>H6/1000000</f>
         <v>0.88481100000000001</v>
       </c>
       <c r="J6" s="15">
-        <f t="shared" si="1"/>
+        <f>I6</f>
         <v>0.88481100000000001</v>
       </c>
       <c r="K6" s="14">
         <v>51</v>
       </c>
       <c r="L6" s="14">
-        <f t="shared" si="2"/>
+        <f>K6</f>
         <v>51</v>
       </c>
       <c r="M6" s="14">
         <v>953</v>
       </c>
       <c r="N6" s="14">
-        <f t="shared" si="3"/>
+        <f>M6</f>
         <v>953</v>
       </c>
       <c r="O6" s="14">
         <v>0.46</v>
       </c>
       <c r="P6" s="14">
-        <f t="shared" si="4"/>
+        <f>O6</f>
         <v>0.46</v>
       </c>
       <c r="Q6" s="14">
         <v>31</v>
       </c>
       <c r="R6" s="15">
-        <f t="shared" si="5"/>
+        <f>Q6/37</f>
         <v>0.83783783783783783</v>
       </c>
       <c r="S6" s="15">
-        <f t="shared" si="8"/>
+        <f>R6</f>
         <v>0.83783783783783783</v>
       </c>
       <c r="T6" s="15">
-        <f t="shared" si="6"/>
+        <f>I6/R6</f>
         <v>1.0560647419354838</v>
       </c>
       <c r="U6" s="15">
-        <f t="shared" si="7"/>
+        <f>T6</f>
         <v>1.0560647419354838</v>
       </c>
       <c r="V6" s="16">
@@ -2772,51 +2772,51 @@
         <v>783186</v>
       </c>
       <c r="I7" s="15">
-        <f t="shared" si="0"/>
+        <f>H7/1000000</f>
         <v>0.78318600000000005</v>
       </c>
       <c r="J7" s="15">
-        <f t="shared" si="1"/>
+        <f>I7</f>
         <v>0.78318600000000005</v>
       </c>
       <c r="K7" s="14">
         <v>54</v>
       </c>
       <c r="L7" s="14">
-        <f t="shared" si="2"/>
+        <f>K7</f>
         <v>54</v>
       </c>
       <c r="M7" s="14">
         <v>848</v>
       </c>
       <c r="N7" s="14">
-        <f t="shared" si="3"/>
+        <f>M7</f>
         <v>848</v>
       </c>
       <c r="O7" s="14">
         <v>0.45</v>
       </c>
       <c r="P7" s="14">
-        <f t="shared" si="4"/>
+        <f>O7</f>
         <v>0.45</v>
       </c>
       <c r="Q7" s="14">
         <v>5</v>
       </c>
       <c r="R7" s="15">
-        <f t="shared" si="5"/>
+        <f>Q7/37</f>
         <v>0.13513513513513514</v>
       </c>
       <c r="S7" s="15">
-        <f t="shared" si="8"/>
+        <f>R7</f>
         <v>0.13513513513513514</v>
       </c>
       <c r="T7" s="15">
-        <f t="shared" si="6"/>
+        <f>I7/R7</f>
         <v>5.7955763999999999</v>
       </c>
       <c r="U7" s="15">
-        <f t="shared" si="7"/>
+        <f>T7</f>
         <v>5.7955763999999999</v>
       </c>
       <c r="V7" s="16">
@@ -2849,51 +2849,51 @@
         <v>695943</v>
       </c>
       <c r="I8" s="15">
-        <f t="shared" si="0"/>
+        <f>H8/1000000</f>
         <v>0.69594299999999998</v>
       </c>
       <c r="J8" s="15">
-        <f t="shared" si="1"/>
+        <f>I8</f>
         <v>0.69594299999999998</v>
       </c>
       <c r="K8" s="14">
         <v>98</v>
       </c>
       <c r="L8" s="14">
-        <f t="shared" si="2"/>
+        <f>K8</f>
         <v>98</v>
       </c>
       <c r="M8" s="14">
         <v>818</v>
       </c>
       <c r="N8" s="14">
-        <f t="shared" si="3"/>
+        <f>M8</f>
         <v>818</v>
       </c>
       <c r="O8" s="14">
         <v>0.45</v>
       </c>
       <c r="P8" s="14">
-        <f t="shared" si="4"/>
+        <f>O8</f>
         <v>0.45</v>
       </c>
       <c r="Q8" s="14">
         <v>4</v>
       </c>
       <c r="R8" s="15">
-        <f t="shared" si="5"/>
+        <f>Q8/37</f>
         <v>0.10810810810810811</v>
       </c>
       <c r="S8" s="15">
-        <f t="shared" si="8"/>
+        <f>R8</f>
         <v>0.10810810810810811</v>
       </c>
       <c r="T8" s="15">
-        <f t="shared" si="6"/>
+        <f>I8/R8</f>
         <v>6.4374727499999995</v>
       </c>
       <c r="U8" s="15">
-        <f t="shared" si="7"/>
+        <f>T8</f>
         <v>6.4374727499999995</v>
       </c>
       <c r="V8" s="16">
@@ -2926,51 +2926,51 @@
         <v>778696</v>
       </c>
       <c r="I9" s="15">
-        <f t="shared" si="0"/>
+        <f>H9/1000000</f>
         <v>0.77869600000000005</v>
       </c>
       <c r="J9" s="15">
-        <f t="shared" si="1"/>
+        <f>I9</f>
         <v>0.77869600000000005</v>
       </c>
       <c r="K9" s="14">
         <v>82</v>
       </c>
       <c r="L9" s="14">
-        <f t="shared" si="2"/>
+        <f>K9</f>
         <v>82</v>
       </c>
       <c r="M9" s="14">
         <v>892</v>
       </c>
       <c r="N9" s="14">
-        <f t="shared" si="3"/>
+        <f>M9</f>
         <v>892</v>
       </c>
       <c r="O9" s="14">
         <v>0.45</v>
       </c>
       <c r="P9" s="14">
-        <f t="shared" si="4"/>
+        <f>O9</f>
         <v>0.45</v>
       </c>
       <c r="Q9" s="14">
         <v>28</v>
       </c>
       <c r="R9" s="15">
-        <f t="shared" si="5"/>
+        <f>Q9/37</f>
         <v>0.7567567567567568</v>
       </c>
       <c r="S9" s="15">
-        <f t="shared" si="8"/>
+        <f>R9</f>
         <v>0.7567567567567568</v>
       </c>
       <c r="T9" s="15">
-        <f t="shared" si="6"/>
+        <f>I9/R9</f>
         <v>1.0289911428571428</v>
       </c>
       <c r="U9" s="15">
-        <f t="shared" si="7"/>
+        <f>T9</f>
         <v>1.0289911428571428</v>
       </c>
       <c r="V9" s="16">
@@ -3003,51 +3003,51 @@
         <v>1381617</v>
       </c>
       <c r="I10" s="15">
-        <f t="shared" si="0"/>
+        <f>H10/1000000</f>
         <v>1.3816170000000001</v>
       </c>
       <c r="J10" s="15">
-        <f t="shared" si="1"/>
+        <f>I10</f>
         <v>1.3816170000000001</v>
       </c>
       <c r="K10" s="14">
         <v>103</v>
       </c>
       <c r="L10" s="14">
-        <f t="shared" si="2"/>
+        <f>K10</f>
         <v>103</v>
       </c>
       <c r="M10" s="14">
         <v>1579</v>
       </c>
       <c r="N10" s="14">
-        <f t="shared" si="3"/>
+        <f>M10</f>
         <v>1579</v>
       </c>
       <c r="O10" s="14">
         <v>0.44</v>
       </c>
       <c r="P10" s="14">
-        <f t="shared" si="4"/>
+        <f>O10</f>
         <v>0.44</v>
       </c>
       <c r="Q10" s="14">
         <v>6</v>
       </c>
       <c r="R10" s="15">
-        <f t="shared" si="5"/>
+        <f>Q10/37</f>
         <v>0.16216216216216217</v>
       </c>
       <c r="S10" s="15">
-        <f t="shared" si="8"/>
+        <f>R10</f>
         <v>0.16216216216216217</v>
       </c>
       <c r="T10" s="15">
-        <f t="shared" si="6"/>
+        <f>I10/R10</f>
         <v>8.5199715000000005</v>
       </c>
       <c r="U10" s="15">
-        <f t="shared" si="7"/>
+        <f>T10</f>
         <v>8.5199715000000005</v>
       </c>
       <c r="V10" s="16">
@@ -3080,51 +3080,51 @@
         <v>1286658</v>
       </c>
       <c r="I11" s="15">
-        <f t="shared" si="0"/>
+        <f>H11/1000000</f>
         <v>1.2866580000000001</v>
       </c>
       <c r="J11" s="15">
-        <f t="shared" si="1"/>
+        <f>I11</f>
         <v>1.2866580000000001</v>
       </c>
       <c r="K11" s="14">
         <v>23</v>
       </c>
       <c r="L11" s="14">
-        <f t="shared" si="2"/>
+        <f>K11</f>
         <v>23</v>
       </c>
       <c r="M11" s="14">
         <v>1341</v>
       </c>
       <c r="N11" s="14">
-        <f t="shared" si="3"/>
+        <f>M11</f>
         <v>1341</v>
       </c>
       <c r="O11" s="14">
         <v>0.46</v>
       </c>
       <c r="P11" s="14">
-        <f t="shared" si="4"/>
+        <f>O11</f>
         <v>0.46</v>
       </c>
       <c r="Q11" s="14">
         <v>16</v>
       </c>
       <c r="R11" s="15">
-        <f t="shared" si="5"/>
+        <f>Q11/37</f>
         <v>0.43243243243243246</v>
       </c>
       <c r="S11" s="15">
-        <f t="shared" si="8"/>
+        <f>R11</f>
         <v>0.43243243243243246</v>
       </c>
       <c r="T11" s="15">
-        <f t="shared" si="6"/>
+        <f>I11/R11</f>
         <v>2.9753966250000001</v>
       </c>
       <c r="U11" s="15">
-        <f t="shared" si="7"/>
+        <f>T11</f>
         <v>2.9753966250000001</v>
       </c>
       <c r="V11" s="16">
@@ -3157,51 +3157,51 @@
         <v>911592</v>
       </c>
       <c r="I12" s="15">
-        <f t="shared" si="0"/>
+        <f>H12/1000000</f>
         <v>0.91159199999999996</v>
       </c>
       <c r="J12" s="15">
-        <f t="shared" si="1"/>
+        <f>I12</f>
         <v>0.91159199999999996</v>
       </c>
       <c r="K12" s="14">
         <v>40</v>
       </c>
       <c r="L12" s="14">
-        <f t="shared" si="2"/>
+        <f>K12</f>
         <v>40</v>
       </c>
       <c r="M12" s="14">
         <v>977</v>
       </c>
       <c r="N12" s="14">
-        <f t="shared" si="3"/>
+        <f>M12</f>
         <v>977</v>
       </c>
       <c r="O12" s="14">
         <v>0.45</v>
       </c>
       <c r="P12" s="14">
-        <f t="shared" si="4"/>
+        <f>O12</f>
         <v>0.45</v>
       </c>
       <c r="Q12" s="14">
         <v>9</v>
       </c>
       <c r="R12" s="15">
-        <f t="shared" si="5"/>
+        <f>Q12/37</f>
         <v>0.24324324324324326</v>
       </c>
       <c r="S12" s="15">
-        <f t="shared" si="8"/>
+        <f>R12</f>
         <v>0.24324324324324326</v>
       </c>
       <c r="T12" s="15">
-        <f t="shared" si="6"/>
+        <f>I12/R12</f>
         <v>3.7476559999999997</v>
       </c>
       <c r="U12" s="15">
-        <f t="shared" si="7"/>
+        <f>T12</f>
         <v>3.7476559999999997</v>
       </c>
       <c r="V12" s="16">
@@ -3234,51 +3234,51 @@
         <v>1366118</v>
       </c>
       <c r="I13" s="15">
-        <f t="shared" si="0"/>
+        <f>H13/1000000</f>
         <v>1.3661179999999999</v>
       </c>
       <c r="J13" s="15">
-        <f t="shared" si="1"/>
+        <f>I13</f>
         <v>1.3661179999999999</v>
       </c>
       <c r="K13" s="14">
         <v>60</v>
       </c>
       <c r="L13" s="14">
-        <f t="shared" si="2"/>
+        <f>K13</f>
         <v>60</v>
       </c>
       <c r="M13" s="14">
         <v>1427</v>
       </c>
       <c r="N13" s="14">
-        <f t="shared" si="3"/>
+        <f>M13</f>
         <v>1427</v>
       </c>
       <c r="O13" s="14">
         <v>0.47</v>
       </c>
       <c r="P13" s="14">
-        <f t="shared" si="4"/>
+        <f>O13</f>
         <v>0.47</v>
       </c>
       <c r="Q13" s="14">
         <v>9</v>
       </c>
       <c r="R13" s="15">
-        <f t="shared" si="5"/>
+        <f>Q13/37</f>
         <v>0.24324324324324326</v>
       </c>
       <c r="S13" s="15">
-        <f t="shared" si="8"/>
+        <f>R13</f>
         <v>0.24324324324324326</v>
       </c>
       <c r="T13" s="15">
-        <f t="shared" si="6"/>
+        <f>I13/R13</f>
         <v>5.6162628888888886</v>
       </c>
       <c r="U13" s="15">
-        <f t="shared" si="7"/>
+        <f>T13</f>
         <v>5.6162628888888886</v>
       </c>
       <c r="V13" s="16">
@@ -3311,51 +3311,51 @@
         <v>753259</v>
       </c>
       <c r="I14" s="15">
-        <f t="shared" si="0"/>
+        <f>H14/1000000</f>
         <v>0.75325900000000001</v>
       </c>
       <c r="J14" s="15">
-        <f t="shared" si="1"/>
+        <f>I14</f>
         <v>0.75325900000000001</v>
       </c>
       <c r="K14" s="14">
         <v>67</v>
       </c>
       <c r="L14" s="14">
-        <f t="shared" si="2"/>
+        <f>K14</f>
         <v>67</v>
       </c>
       <c r="M14" s="14">
         <v>827</v>
       </c>
       <c r="N14" s="14">
-        <f t="shared" si="3"/>
+        <f>M14</f>
         <v>827</v>
       </c>
       <c r="O14" s="14">
         <v>0.4</v>
       </c>
       <c r="P14" s="14">
-        <f t="shared" si="4"/>
+        <f>O14</f>
         <v>0.4</v>
       </c>
       <c r="Q14" s="14">
         <v>16</v>
       </c>
       <c r="R14" s="15">
-        <f t="shared" si="5"/>
+        <f>Q14/37</f>
         <v>0.43243243243243246</v>
       </c>
       <c r="S14" s="15">
-        <f t="shared" si="8"/>
+        <f>R14</f>
         <v>0.43243243243243246</v>
       </c>
       <c r="T14" s="15">
-        <f t="shared" si="6"/>
+        <f>I14/R14</f>
         <v>1.7419114375</v>
       </c>
       <c r="U14" s="15">
-        <f t="shared" si="7"/>
+        <f>T14</f>
         <v>1.7419114375</v>
       </c>
       <c r="V14" s="16">
@@ -3388,51 +3388,51 @@
         <v>966755</v>
       </c>
       <c r="I15" s="15">
-        <f t="shared" si="0"/>
+        <f>H15/1000000</f>
         <v>0.96675500000000003</v>
       </c>
       <c r="J15" s="15">
-        <f t="shared" si="1"/>
+        <f>I15</f>
         <v>0.96675500000000003</v>
       </c>
       <c r="K15" s="14">
         <v>81</v>
       </c>
       <c r="L15" s="14">
-        <f t="shared" si="2"/>
+        <f>K15</f>
         <v>81</v>
       </c>
       <c r="M15" s="14">
         <v>1094</v>
       </c>
       <c r="N15" s="14">
-        <f t="shared" si="3"/>
+        <f>M15</f>
         <v>1094</v>
       </c>
       <c r="O15" s="14">
         <v>0.42</v>
       </c>
       <c r="P15" s="14">
-        <f t="shared" si="4"/>
+        <f>O15</f>
         <v>0.42</v>
       </c>
       <c r="Q15" s="14">
         <v>32</v>
       </c>
       <c r="R15" s="15">
-        <f t="shared" si="5"/>
+        <f>Q15/37</f>
         <v>0.86486486486486491</v>
       </c>
       <c r="S15" s="15">
-        <f t="shared" si="8"/>
+        <f>R15</f>
         <v>0.86486486486486491</v>
       </c>
       <c r="T15" s="15">
-        <f t="shared" si="6"/>
+        <f>I15/R15</f>
         <v>1.1178104687499999</v>
       </c>
       <c r="U15" s="15">
-        <f t="shared" si="7"/>
+        <f>T15</f>
         <v>1.1178104687499999</v>
       </c>
       <c r="V15" s="16">
@@ -3465,51 +3465,51 @@
         <v>1163583</v>
       </c>
       <c r="I16" s="15">
-        <f t="shared" si="0"/>
+        <f>H16/1000000</f>
         <v>1.163583</v>
       </c>
       <c r="J16" s="15">
-        <f t="shared" si="1"/>
+        <f>I16</f>
         <v>1.163583</v>
       </c>
       <c r="K16" s="14">
         <v>75</v>
       </c>
       <c r="L16" s="14">
-        <f t="shared" si="2"/>
+        <f>K16</f>
         <v>75</v>
       </c>
       <c r="M16" s="14">
         <v>1282</v>
       </c>
       <c r="N16" s="14">
-        <f t="shared" si="3"/>
+        <f>M16</f>
         <v>1282</v>
       </c>
       <c r="O16" s="14">
         <v>0.42</v>
       </c>
       <c r="P16" s="14">
-        <f t="shared" si="4"/>
+        <f>O16</f>
         <v>0.42</v>
       </c>
       <c r="Q16" s="14">
         <v>36</v>
       </c>
       <c r="R16" s="15">
-        <f t="shared" si="5"/>
+        <f>Q16/37</f>
         <v>0.97297297297297303</v>
       </c>
       <c r="S16" s="15">
-        <f t="shared" si="8"/>
+        <f>R16</f>
         <v>0.97297297297297303</v>
       </c>
       <c r="T16" s="15">
-        <f t="shared" si="6"/>
+        <f>I16/R16</f>
         <v>1.19590475</v>
       </c>
       <c r="U16" s="15">
-        <f t="shared" si="7"/>
+        <f>T16</f>
         <v>1.19590475</v>
       </c>
       <c r="V16" s="16">
@@ -3542,51 +3542,51 @@
         <v>833294</v>
       </c>
       <c r="I17" s="15">
-        <f t="shared" si="0"/>
+        <f>H17/1000000</f>
         <v>0.83329399999999998</v>
       </c>
       <c r="J17" s="15">
-        <f t="shared" si="1"/>
+        <f>I17</f>
         <v>0.83329399999999998</v>
       </c>
       <c r="K17" s="14">
         <v>64</v>
       </c>
       <c r="L17" s="14">
-        <f t="shared" si="2"/>
+        <f>K17</f>
         <v>64</v>
       </c>
       <c r="M17" s="14">
         <v>913</v>
       </c>
       <c r="N17" s="14">
-        <f t="shared" si="3"/>
+        <f>M17</f>
         <v>913</v>
       </c>
       <c r="O17" s="14">
         <v>0.42</v>
       </c>
       <c r="P17" s="14">
-        <f t="shared" si="4"/>
+        <f>O17</f>
         <v>0.42</v>
       </c>
       <c r="Q17" s="14">
         <v>30</v>
       </c>
       <c r="R17" s="15">
-        <f t="shared" si="5"/>
+        <f>Q17/37</f>
         <v>0.81081081081081086</v>
       </c>
       <c r="S17" s="15">
-        <f t="shared" si="8"/>
+        <f>R17</f>
         <v>0.81081081081081086</v>
       </c>
       <c r="T17" s="15">
-        <f t="shared" si="6"/>
+        <f>I17/R17</f>
         <v>1.0277292666666666</v>
       </c>
       <c r="U17" s="15">
-        <f t="shared" si="7"/>
+        <f>T17</f>
         <v>1.0277292666666666</v>
       </c>
       <c r="V17" s="16">
@@ -3619,51 +3619,51 @@
         <v>944397</v>
       </c>
       <c r="I18" s="15">
-        <f t="shared" si="0"/>
+        <f>H18/1000000</f>
         <v>0.94439700000000004</v>
       </c>
       <c r="J18" s="15">
-        <f t="shared" si="1"/>
+        <f>I18</f>
         <v>0.94439700000000004</v>
       </c>
       <c r="K18" s="14">
         <v>54</v>
       </c>
       <c r="L18" s="14">
-        <f t="shared" si="2"/>
+        <f>K18</f>
         <v>54</v>
       </c>
       <c r="M18" s="14">
         <v>1037</v>
       </c>
       <c r="N18" s="14">
-        <f t="shared" si="3"/>
+        <f>M18</f>
         <v>1037</v>
       </c>
       <c r="O18" s="14">
         <v>0.41</v>
       </c>
       <c r="P18" s="14">
-        <f t="shared" si="4"/>
+        <f>O18</f>
         <v>0.41</v>
       </c>
       <c r="Q18" s="14">
         <v>14</v>
       </c>
       <c r="R18" s="15">
-        <f t="shared" si="5"/>
+        <f>Q18/37</f>
         <v>0.3783783783783784</v>
       </c>
       <c r="S18" s="15">
-        <f t="shared" si="8"/>
+        <f>R18</f>
         <v>0.3783783783783784</v>
       </c>
       <c r="T18" s="15">
-        <f t="shared" si="6"/>
+        <f>I18/R18</f>
         <v>2.4959063571428572</v>
       </c>
       <c r="U18" s="15">
-        <f t="shared" si="7"/>
+        <f>T18</f>
         <v>2.4959063571428572</v>
       </c>
       <c r="V18" s="16">
@@ -3696,51 +3696,51 @@
         <v>660403</v>
       </c>
       <c r="I19" s="15">
-        <f t="shared" si="0"/>
+        <f>H19/1000000</f>
         <v>0.66040299999999996</v>
       </c>
       <c r="J19" s="15">
-        <f t="shared" si="1"/>
+        <f>I19</f>
         <v>0.66040299999999996</v>
       </c>
       <c r="K19" s="14">
         <v>66</v>
       </c>
       <c r="L19" s="14">
-        <f t="shared" si="2"/>
+        <f>K19</f>
         <v>66</v>
       </c>
       <c r="M19" s="14">
         <v>736</v>
       </c>
       <c r="N19" s="14">
-        <f t="shared" si="3"/>
+        <f>M19</f>
         <v>736</v>
       </c>
       <c r="O19" s="14">
         <v>0.41</v>
       </c>
       <c r="P19" s="14">
-        <f t="shared" si="4"/>
+        <f>O19</f>
         <v>0.41</v>
       </c>
       <c r="Q19" s="14">
         <v>5</v>
       </c>
       <c r="R19" s="15">
-        <f t="shared" si="5"/>
+        <f>Q19/37</f>
         <v>0.13513513513513514</v>
       </c>
       <c r="S19" s="15">
-        <f t="shared" si="8"/>
+        <f>R19</f>
         <v>0.13513513513513514</v>
       </c>
       <c r="T19" s="15">
-        <f t="shared" si="6"/>
+        <f>I19/R19</f>
         <v>4.8869821999999994</v>
       </c>
       <c r="U19" s="15">
-        <f t="shared" si="7"/>
+        <f>T19</f>
         <v>4.8869821999999994</v>
       </c>
       <c r="V19" s="16">
@@ -3773,51 +3773,51 @@
         <v>734855</v>
       </c>
       <c r="I20" s="15">
-        <f t="shared" si="0"/>
+        <f>H20/1000000</f>
         <v>0.73485500000000004</v>
       </c>
       <c r="J20" s="15">
-        <f t="shared" si="1"/>
+        <f>I20</f>
         <v>0.73485500000000004</v>
       </c>
       <c r="K20" s="14">
         <v>58</v>
       </c>
       <c r="L20" s="14">
-        <f t="shared" si="2"/>
+        <f>K20</f>
         <v>58</v>
       </c>
       <c r="M20" s="14">
         <v>804</v>
       </c>
       <c r="N20" s="14">
-        <f t="shared" si="3"/>
+        <f>M20</f>
         <v>804</v>
       </c>
       <c r="O20" s="14">
         <v>0.4</v>
       </c>
       <c r="P20" s="14">
-        <f t="shared" si="4"/>
+        <f>O20</f>
         <v>0.4</v>
       </c>
       <c r="Q20" s="14">
         <v>14</v>
       </c>
       <c r="R20" s="15">
-        <f t="shared" si="5"/>
+        <f>Q20/37</f>
         <v>0.3783783783783784</v>
       </c>
       <c r="S20" s="15">
-        <f t="shared" si="8"/>
+        <f>R20</f>
         <v>0.3783783783783784</v>
       </c>
       <c r="T20" s="15">
-        <f t="shared" si="6"/>
+        <f>I20/R20</f>
         <v>1.9421167857142858</v>
       </c>
       <c r="U20" s="15">
-        <f t="shared" si="7"/>
+        <f>T20</f>
         <v>1.9421167857142858</v>
       </c>
       <c r="V20" s="16">
@@ -3850,51 +3850,51 @@
         <v>1154578</v>
       </c>
       <c r="I21" s="15">
-        <f t="shared" si="0"/>
+        <f>H21/1000000</f>
         <v>1.1545780000000001</v>
       </c>
       <c r="J21" s="15">
-        <f t="shared" si="1"/>
+        <f>I21</f>
         <v>1.1545780000000001</v>
       </c>
       <c r="K21" s="14">
         <v>30</v>
       </c>
       <c r="L21" s="14">
-        <f t="shared" si="2"/>
+        <f>K21</f>
         <v>30</v>
       </c>
       <c r="M21" s="14">
         <v>1214</v>
       </c>
       <c r="N21" s="14">
-        <f t="shared" si="3"/>
+        <f>M21</f>
         <v>1214</v>
       </c>
       <c r="O21" s="14">
         <v>0.44</v>
       </c>
       <c r="P21" s="14">
-        <f t="shared" si="4"/>
+        <f>O21</f>
         <v>0.44</v>
       </c>
       <c r="Q21" s="14">
         <v>35</v>
       </c>
       <c r="R21" s="15">
-        <f t="shared" si="5"/>
+        <f>Q21/37</f>
         <v>0.94594594594594594</v>
       </c>
       <c r="S21" s="15">
-        <f t="shared" si="8"/>
+        <f>R21</f>
         <v>0.94594594594594594</v>
       </c>
       <c r="T21" s="15">
-        <f t="shared" si="6"/>
+        <f>I21/R21</f>
         <v>1.2205538857142859</v>
       </c>
       <c r="U21" s="15">
-        <f t="shared" si="7"/>
+        <f>T21</f>
         <v>1.2205538857142859</v>
       </c>
       <c r="V21" s="16">
@@ -3927,51 +3927,51 @@
         <v>1144269</v>
       </c>
       <c r="I22" s="15">
-        <f t="shared" si="0"/>
+        <f>H22/1000000</f>
         <v>1.144269</v>
       </c>
       <c r="J22" s="15">
-        <f t="shared" si="1"/>
+        <f>I22</f>
         <v>1.144269</v>
       </c>
       <c r="K22" s="14">
         <v>99</v>
       </c>
       <c r="L22" s="14">
-        <f t="shared" si="2"/>
+        <f>K22</f>
         <v>99</v>
       </c>
       <c r="M22" s="14">
         <v>1209</v>
       </c>
       <c r="N22" s="14">
-        <f t="shared" si="3"/>
+        <f>M22</f>
         <v>1209</v>
       </c>
       <c r="O22" s="14">
         <v>0.45</v>
       </c>
       <c r="P22" s="14">
-        <f t="shared" si="4"/>
+        <f>O22</f>
         <v>0.45</v>
       </c>
       <c r="Q22" s="14">
         <v>9</v>
       </c>
       <c r="R22" s="15">
-        <f t="shared" si="5"/>
+        <f>Q22/37</f>
         <v>0.24324324324324326</v>
       </c>
       <c r="S22" s="15">
-        <f t="shared" si="8"/>
+        <f>R22</f>
         <v>0.24324324324324326</v>
       </c>
       <c r="T22" s="15">
-        <f t="shared" si="6"/>
+        <f>I22/R22</f>
         <v>4.7042169999999999</v>
       </c>
       <c r="U22" s="15">
-        <f t="shared" si="7"/>
+        <f>T22</f>
         <v>4.7042169999999999</v>
       </c>
       <c r="V22" s="16">
@@ -4004,51 +4004,51 @@
         <v>971617</v>
       </c>
       <c r="I23" s="15">
-        <f t="shared" si="0"/>
+        <f>H23/1000000</f>
         <v>0.97161699999999995</v>
       </c>
       <c r="J23" s="15">
-        <f t="shared" si="1"/>
+        <f>I23</f>
         <v>0.97161699999999995</v>
       </c>
       <c r="K23" s="14">
         <v>97</v>
       </c>
       <c r="L23" s="14">
-        <f t="shared" si="2"/>
+        <f>K23</f>
         <v>97</v>
       </c>
       <c r="M23" s="14">
         <v>1063</v>
       </c>
       <c r="N23" s="14">
-        <f t="shared" si="3"/>
+        <f>M23</f>
         <v>1063</v>
       </c>
       <c r="O23" s="14">
         <v>0.5</v>
       </c>
       <c r="P23" s="14">
-        <f t="shared" si="4"/>
+        <f>O23</f>
         <v>0.5</v>
       </c>
       <c r="Q23" s="14">
         <v>12</v>
       </c>
       <c r="R23" s="15">
-        <f t="shared" si="5"/>
+        <f>Q23/37</f>
         <v>0.32432432432432434</v>
       </c>
       <c r="S23" s="15">
-        <f t="shared" si="8"/>
+        <f>R23</f>
         <v>0.32432432432432434</v>
       </c>
       <c r="T23" s="15">
-        <f t="shared" si="6"/>
+        <f>I23/R23</f>
         <v>2.9958190833333331</v>
       </c>
       <c r="U23" s="15">
-        <f t="shared" si="7"/>
+        <f>T23</f>
         <v>2.9958190833333331</v>
       </c>
       <c r="V23" s="16">
@@ -4081,51 +4081,51 @@
         <v>1361355</v>
       </c>
       <c r="I24" s="15">
-        <f t="shared" si="0"/>
+        <f>H24/1000000</f>
         <v>1.3613550000000001</v>
       </c>
       <c r="J24" s="15">
-        <f t="shared" si="1"/>
+        <f>I24</f>
         <v>1.3613550000000001</v>
       </c>
       <c r="K24" s="14">
         <v>73</v>
       </c>
       <c r="L24" s="14">
-        <f t="shared" si="2"/>
+        <f>K24</f>
         <v>73</v>
       </c>
       <c r="M24" s="14">
         <v>1441</v>
       </c>
       <c r="N24" s="14">
-        <f t="shared" si="3"/>
+        <f>M24</f>
         <v>1441</v>
       </c>
       <c r="O24" s="14">
         <v>0.5</v>
       </c>
       <c r="P24" s="14">
-        <f t="shared" si="4"/>
+        <f>O24</f>
         <v>0.5</v>
       </c>
       <c r="Q24" s="14">
         <v>12</v>
       </c>
       <c r="R24" s="15">
-        <f t="shared" si="5"/>
+        <f>Q24/37</f>
         <v>0.32432432432432434</v>
       </c>
       <c r="S24" s="15">
-        <f t="shared" si="8"/>
+        <f>R24</f>
         <v>0.32432432432432434</v>
       </c>
       <c r="T24" s="15">
-        <f t="shared" si="6"/>
+        <f>I24/R24</f>
         <v>4.1975112499999998</v>
       </c>
       <c r="U24" s="15">
-        <f t="shared" si="7"/>
+        <f>T24</f>
         <v>4.1975112499999998</v>
       </c>
       <c r="V24" s="16">
@@ -4158,51 +4158,51 @@
         <v>1245790</v>
       </c>
       <c r="I25" s="15">
-        <f t="shared" si="0"/>
+        <f>H25/1000000</f>
         <v>1.24579</v>
       </c>
       <c r="J25" s="15">
-        <f t="shared" si="1"/>
+        <f>I25</f>
         <v>1.24579</v>
       </c>
       <c r="K25" s="14">
         <v>119</v>
       </c>
       <c r="L25" s="14">
-        <f t="shared" si="2"/>
+        <f>K25</f>
         <v>119</v>
       </c>
       <c r="M25" s="14">
         <v>1338</v>
       </c>
       <c r="N25" s="14">
-        <f t="shared" si="3"/>
+        <f>M25</f>
         <v>1338</v>
       </c>
       <c r="O25" s="14">
         <v>0.47</v>
       </c>
       <c r="P25" s="14">
-        <f t="shared" si="4"/>
+        <f>O25</f>
         <v>0.47</v>
       </c>
       <c r="Q25" s="14">
         <v>15</v>
       </c>
       <c r="R25" s="15">
-        <f t="shared" si="5"/>
+        <f>Q25/37</f>
         <v>0.40540540540540543</v>
       </c>
       <c r="S25" s="15">
-        <f t="shared" si="8"/>
+        <f>R25</f>
         <v>0.40540540540540543</v>
       </c>
       <c r="T25" s="15">
-        <f t="shared" si="6"/>
+        <f>I25/R25</f>
         <v>3.0729486666666666</v>
       </c>
       <c r="U25" s="15">
-        <f t="shared" si="7"/>
+        <f>T25</f>
         <v>3.0729486666666666</v>
       </c>
       <c r="V25" s="16">
@@ -4235,51 +4235,51 @@
         <v>949240</v>
       </c>
       <c r="I26" s="15">
-        <f t="shared" si="0"/>
+        <f>H26/1000000</f>
         <v>0.94923999999999997</v>
       </c>
       <c r="J26" s="15">
-        <f t="shared" si="1"/>
+        <f>I26</f>
         <v>0.94923999999999997</v>
       </c>
       <c r="K26" s="14">
         <v>105</v>
       </c>
       <c r="L26" s="14">
-        <f t="shared" si="2"/>
+        <f>K26</f>
         <v>105</v>
       </c>
       <c r="M26" s="14">
         <v>1031</v>
       </c>
       <c r="N26" s="14">
-        <f t="shared" si="3"/>
+        <f>M26</f>
         <v>1031</v>
       </c>
       <c r="O26" s="14">
         <v>0.51</v>
       </c>
       <c r="P26" s="14">
-        <f t="shared" si="4"/>
+        <f>O26</f>
         <v>0.51</v>
       </c>
       <c r="Q26" s="14">
         <v>11</v>
       </c>
       <c r="R26" s="15">
-        <f t="shared" si="5"/>
+        <f>Q26/37</f>
         <v>0.29729729729729731</v>
       </c>
       <c r="S26" s="15">
-        <f t="shared" si="8"/>
+        <f>R26</f>
         <v>0.29729729729729731</v>
       </c>
       <c r="T26" s="15">
-        <f t="shared" si="6"/>
+        <f>I26/R26</f>
         <v>3.1928981818181814</v>
       </c>
       <c r="U26" s="15">
-        <f t="shared" si="7"/>
+        <f>T26</f>
         <v>3.1928981818181814</v>
       </c>
       <c r="V26" s="16">
@@ -4312,51 +4312,51 @@
         <v>992136</v>
       </c>
       <c r="I27" s="15">
-        <f t="shared" si="0"/>
+        <f>H27/1000000</f>
         <v>0.99213600000000002</v>
       </c>
       <c r="J27" s="15">
-        <f t="shared" si="1"/>
+        <f>I27</f>
         <v>0.99213600000000002</v>
       </c>
       <c r="K27" s="14">
         <v>99</v>
       </c>
       <c r="L27" s="14">
-        <f t="shared" si="2"/>
+        <f>K27</f>
         <v>99</v>
       </c>
       <c r="M27" s="14">
         <v>1081</v>
       </c>
       <c r="N27" s="14">
-        <f t="shared" si="3"/>
+        <f>M27</f>
         <v>1081</v>
       </c>
       <c r="O27" s="14">
         <v>0.46</v>
       </c>
       <c r="P27" s="14">
-        <f t="shared" si="4"/>
+        <f>O27</f>
         <v>0.46</v>
       </c>
       <c r="Q27" s="14">
         <v>7</v>
       </c>
       <c r="R27" s="15">
-        <f t="shared" si="5"/>
+        <f>Q27/37</f>
         <v>0.1891891891891892</v>
       </c>
       <c r="S27" s="15">
-        <f t="shared" si="8"/>
+        <f>R27</f>
         <v>0.1891891891891892</v>
       </c>
       <c r="T27" s="15">
-        <f t="shared" si="6"/>
+        <f>I27/R27</f>
         <v>5.244147428571428</v>
       </c>
       <c r="U27" s="15">
-        <f t="shared" si="7"/>
+        <f>T27</f>
         <v>5.244147428571428</v>
       </c>
       <c r="V27" s="16">
@@ -4389,51 +4389,51 @@
         <v>845311</v>
       </c>
       <c r="I28" s="15">
-        <f t="shared" si="0"/>
+        <f>H28/1000000</f>
         <v>0.84531100000000003</v>
       </c>
       <c r="J28" s="15">
-        <f t="shared" si="1"/>
+        <f>I28</f>
         <v>0.84531100000000003</v>
       </c>
       <c r="K28" s="14">
         <v>113</v>
       </c>
       <c r="L28" s="14">
-        <f t="shared" si="2"/>
+        <f>K28</f>
         <v>113</v>
       </c>
       <c r="M28" s="14">
         <v>980</v>
       </c>
       <c r="N28" s="14">
-        <f t="shared" si="3"/>
+        <f>M28</f>
         <v>980</v>
       </c>
       <c r="O28" s="14">
         <v>0.46</v>
       </c>
       <c r="P28" s="14">
-        <f t="shared" si="4"/>
+        <f>O28</f>
         <v>0.46</v>
       </c>
       <c r="Q28" s="14">
         <v>14</v>
       </c>
       <c r="R28" s="15">
-        <f t="shared" si="5"/>
+        <f>Q28/37</f>
         <v>0.3783783783783784</v>
       </c>
       <c r="S28" s="15">
-        <f t="shared" si="8"/>
+        <f>R28</f>
         <v>0.3783783783783784</v>
       </c>
       <c r="T28" s="15">
-        <f t="shared" si="6"/>
+        <f>I28/R28</f>
         <v>2.2340362142857142</v>
       </c>
       <c r="U28" s="15">
-        <f t="shared" si="7"/>
+        <f>T28</f>
         <v>2.2340362142857142</v>
       </c>
       <c r="V28" s="16">
@@ -4466,51 +4466,51 @@
         <v>1214182</v>
       </c>
       <c r="I29" s="15">
-        <f t="shared" si="0"/>
+        <f>H29/1000000</f>
         <v>1.2141820000000001</v>
       </c>
       <c r="J29" s="15">
-        <f t="shared" si="1"/>
+        <f>I29</f>
         <v>1.2141820000000001</v>
       </c>
       <c r="K29" s="14">
         <v>125</v>
       </c>
       <c r="L29" s="14">
-        <f t="shared" si="2"/>
+        <f>K29</f>
         <v>125</v>
       </c>
       <c r="M29" s="14">
         <v>1314</v>
       </c>
       <c r="N29" s="14">
-        <f t="shared" si="3"/>
+        <f>M29</f>
         <v>1314</v>
       </c>
       <c r="O29" s="14">
         <v>0.47</v>
       </c>
       <c r="P29" s="14">
-        <f t="shared" si="4"/>
+        <f>O29</f>
         <v>0.47</v>
       </c>
       <c r="Q29" s="14">
         <v>34</v>
       </c>
       <c r="R29" s="15">
-        <f t="shared" si="5"/>
+        <f>Q29/37</f>
         <v>0.91891891891891897</v>
       </c>
       <c r="S29" s="15">
-        <f t="shared" si="8"/>
+        <f>R29</f>
         <v>0.91891891891891897</v>
       </c>
       <c r="T29" s="15">
-        <f t="shared" si="6"/>
+        <f>I29/R29</f>
         <v>1.321315705882353</v>
       </c>
       <c r="U29" s="15">
-        <f t="shared" si="7"/>
+        <f>T29</f>
         <v>1.321315705882353</v>
       </c>
       <c r="V29" s="16">
@@ -4543,51 +4543,51 @@
         <v>468462</v>
       </c>
       <c r="I30" s="15">
-        <f t="shared" si="0"/>
+        <f>H30/1000000</f>
         <v>0.46846199999999999</v>
       </c>
       <c r="J30" s="15">
-        <f t="shared" si="1"/>
+        <f>I30</f>
         <v>0.46846199999999999</v>
       </c>
       <c r="K30" s="14">
         <v>54</v>
       </c>
       <c r="L30" s="14">
-        <f t="shared" si="2"/>
+        <f>K30</f>
         <v>54</v>
       </c>
       <c r="M30" s="14">
         <v>514</v>
       </c>
       <c r="N30" s="14">
-        <f t="shared" si="3"/>
+        <f>M30</f>
         <v>514</v>
       </c>
       <c r="O30" s="14">
         <v>0.5</v>
       </c>
       <c r="P30" s="14">
-        <f t="shared" si="4"/>
+        <f>O30</f>
         <v>0.5</v>
       </c>
       <c r="Q30" s="14">
         <v>4</v>
       </c>
       <c r="R30" s="15">
-        <f t="shared" si="5"/>
+        <f>Q30/37</f>
         <v>0.10810810810810811</v>
       </c>
       <c r="S30" s="15">
-        <f t="shared" si="8"/>
+        <f>R30</f>
         <v>0.10810810810810811</v>
       </c>
       <c r="T30" s="15">
-        <f t="shared" si="6"/>
+        <f>I30/R30</f>
         <v>4.3332734999999998</v>
       </c>
       <c r="U30" s="15">
-        <f t="shared" si="7"/>
+        <f>T30</f>
         <v>4.3332734999999998</v>
       </c>
       <c r="V30" s="16">
@@ -4620,51 +4620,51 @@
         <v>1257796</v>
       </c>
       <c r="I31" s="15">
-        <f t="shared" si="0"/>
+        <f>H31/1000000</f>
         <v>1.2577959999999999</v>
       </c>
       <c r="J31" s="15">
-        <f t="shared" si="1"/>
+        <f>I31</f>
         <v>1.2577959999999999</v>
       </c>
       <c r="K31" s="14">
         <v>81</v>
       </c>
       <c r="L31" s="14">
-        <f t="shared" si="2"/>
+        <f>K31</f>
         <v>81</v>
       </c>
       <c r="M31" s="14">
         <v>1353</v>
       </c>
       <c r="N31" s="14">
-        <f t="shared" si="3"/>
+        <f>M31</f>
         <v>1353</v>
       </c>
       <c r="O31" s="14">
         <v>0.5</v>
       </c>
       <c r="P31" s="14">
-        <f t="shared" si="4"/>
+        <f>O31</f>
         <v>0.5</v>
       </c>
       <c r="Q31" s="14">
         <v>7</v>
       </c>
       <c r="R31" s="15">
-        <f t="shared" si="5"/>
+        <f>Q31/37</f>
         <v>0.1891891891891892</v>
       </c>
       <c r="S31" s="15">
-        <f t="shared" si="8"/>
+        <f>R31</f>
         <v>0.1891891891891892</v>
       </c>
       <c r="T31" s="15">
-        <f t="shared" si="6"/>
+        <f>I31/R31</f>
         <v>6.6483502857142849</v>
       </c>
       <c r="U31" s="15">
-        <f t="shared" si="7"/>
+        <f>T31</f>
         <v>6.6483502857142849</v>
       </c>
       <c r="V31" s="16">
@@ -4697,51 +4697,51 @@
         <v>786155</v>
       </c>
       <c r="I32" s="15">
-        <f t="shared" si="0"/>
+        <f>H32/1000000</f>
         <v>0.78615500000000005</v>
       </c>
       <c r="J32" s="15">
-        <f t="shared" si="1"/>
+        <f>I32</f>
         <v>0.78615500000000005</v>
       </c>
       <c r="K32" s="14">
         <v>70</v>
       </c>
       <c r="L32" s="14">
-        <f t="shared" si="2"/>
+        <f>K32</f>
         <v>70</v>
       </c>
       <c r="M32" s="14">
         <v>839</v>
       </c>
       <c r="N32" s="14">
-        <f t="shared" si="3"/>
+        <f>M32</f>
         <v>839</v>
       </c>
       <c r="O32" s="14">
         <v>0.48</v>
       </c>
       <c r="P32" s="14">
-        <f t="shared" si="4"/>
+        <f>O32</f>
         <v>0.48</v>
       </c>
       <c r="Q32" s="14">
         <v>10</v>
       </c>
       <c r="R32" s="15">
-        <f t="shared" si="5"/>
+        <f>Q32/37</f>
         <v>0.27027027027027029</v>
       </c>
       <c r="S32" s="15">
-        <f t="shared" si="8"/>
+        <f>R32</f>
         <v>0.27027027027027029</v>
       </c>
       <c r="T32" s="15">
-        <f t="shared" si="6"/>
+        <f>I32/R32</f>
         <v>2.9087735000000001</v>
       </c>
       <c r="U32" s="15">
-        <f t="shared" si="7"/>
+        <f>T32</f>
         <v>2.9087735000000001</v>
       </c>
       <c r="V32" s="16">
@@ -4774,51 +4774,51 @@
         <v>866493</v>
       </c>
       <c r="I33" s="15">
-        <f t="shared" si="0"/>
+        <f>H33/1000000</f>
         <v>0.86649299999999996</v>
       </c>
       <c r="J33" s="15">
-        <f t="shared" si="1"/>
+        <f>I33</f>
         <v>0.86649299999999996</v>
       </c>
       <c r="K33" s="14">
         <v>78</v>
       </c>
       <c r="L33" s="14">
-        <f t="shared" si="2"/>
+        <f>K33</f>
         <v>78</v>
       </c>
       <c r="M33" s="14">
         <v>906</v>
       </c>
       <c r="N33" s="14">
-        <f t="shared" si="3"/>
+        <f>M33</f>
         <v>906</v>
       </c>
       <c r="O33" s="14">
         <v>0.44</v>
       </c>
       <c r="P33" s="14">
-        <f t="shared" si="4"/>
+        <f>O33</f>
         <v>0.44</v>
       </c>
       <c r="Q33" s="14">
         <v>7</v>
       </c>
       <c r="R33" s="15">
-        <f t="shared" si="5"/>
+        <f>Q33/37</f>
         <v>0.1891891891891892</v>
       </c>
       <c r="S33" s="15">
-        <f t="shared" si="8"/>
+        <f>R33</f>
         <v>0.1891891891891892</v>
       </c>
       <c r="T33" s="15">
-        <f t="shared" si="6"/>
+        <f>I33/R33</f>
         <v>4.5800344285714285</v>
       </c>
       <c r="U33" s="15">
-        <f t="shared" si="7"/>
+        <f>T33</f>
         <v>4.5800344285714285</v>
       </c>
       <c r="V33" s="16">
@@ -4851,51 +4851,51 @@
         <v>768848</v>
       </c>
       <c r="I34" s="15">
-        <f t="shared" ref="I34:I56" si="9">H34/1000000</f>
+        <f>H34/1000000</f>
         <v>0.76884799999999998</v>
       </c>
       <c r="J34" s="15">
-        <f t="shared" ref="J34:J56" si="10">I34</f>
+        <f>I34</f>
         <v>0.76884799999999998</v>
       </c>
       <c r="K34" s="14">
         <v>43</v>
       </c>
       <c r="L34" s="14">
-        <f t="shared" ref="L34:L56" si="11">K34</f>
+        <f>K34</f>
         <v>43</v>
       </c>
       <c r="M34" s="14">
         <v>821</v>
       </c>
       <c r="N34" s="14">
-        <f t="shared" ref="N34:N56" si="12">M34</f>
+        <f>M34</f>
         <v>821</v>
       </c>
       <c r="O34" s="14">
         <v>0.53</v>
       </c>
       <c r="P34" s="14">
-        <f t="shared" ref="P34:P56" si="13">O34</f>
+        <f>O34</f>
         <v>0.53</v>
       </c>
       <c r="Q34" s="14">
         <v>22</v>
       </c>
       <c r="R34" s="15">
-        <f t="shared" ref="R34:R56" si="14">Q34/37</f>
+        <f>Q34/37</f>
         <v>0.59459459459459463</v>
       </c>
       <c r="S34" s="15">
-        <f t="shared" si="8"/>
+        <f>R34</f>
         <v>0.59459459459459463</v>
       </c>
       <c r="T34" s="15">
-        <f t="shared" ref="T34:T56" si="15">I34/R34</f>
+        <f>I34/R34</f>
         <v>1.2930625454545452</v>
       </c>
       <c r="U34" s="15">
-        <f t="shared" ref="U34:U56" si="16">T34</f>
+        <f>T34</f>
         <v>1.2930625454545452</v>
       </c>
       <c r="V34" s="16">
@@ -4928,43 +4928,43 @@
         <v>1026123</v>
       </c>
       <c r="I35" s="15">
-        <f t="shared" si="9"/>
+        <f>H35/1000000</f>
         <v>1.0261229999999999</v>
       </c>
       <c r="J35" s="15">
-        <f t="shared" si="10"/>
+        <f>I35</f>
         <v>1.0261229999999999</v>
       </c>
       <c r="K35" s="14">
         <v>58</v>
       </c>
       <c r="L35" s="14">
-        <f t="shared" si="11"/>
+        <f>K35</f>
         <v>58</v>
       </c>
       <c r="M35" s="14">
         <v>1075</v>
       </c>
       <c r="N35" s="14">
-        <f t="shared" si="12"/>
+        <f>M35</f>
         <v>1075</v>
       </c>
       <c r="O35" s="14">
         <v>0.5</v>
       </c>
       <c r="P35" s="14">
-        <f t="shared" si="13"/>
+        <f>O35</f>
         <v>0.5</v>
       </c>
       <c r="Q35" s="14">
         <v>29</v>
       </c>
       <c r="R35" s="15">
-        <f t="shared" si="14"/>
+        <f>Q35/37</f>
         <v>0.78378378378378377</v>
       </c>
       <c r="S35" s="15">
-        <f t="shared" si="8"/>
+        <f>R35</f>
         <v>0.78378378378378377</v>
       </c>
       <c r="T35" s="15">
@@ -4981,13 +4981,13 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="13" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>243</v>
+        <v>31</v>
       </c>
       <c r="C36" s="14">
-        <v>2619619040</v>
+        <v>2582580539</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>119</v>
@@ -4996,152 +4996,152 @@
         <v>122</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>188</v>
+        <v>123</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="H36" s="14">
-        <v>427469</v>
+        <v>1793743</v>
       </c>
       <c r="I36" s="15">
-        <f t="shared" si="9"/>
-        <v>0.42746899999999999</v>
+        <f>H36/1000000</f>
+        <v>1.7937430000000001</v>
       </c>
       <c r="J36" s="15">
-        <f t="shared" si="10"/>
-        <v>0.42746899999999999</v>
+        <f>I36</f>
+        <v>1.7937430000000001</v>
       </c>
       <c r="K36" s="14">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="L36" s="14">
-        <f t="shared" si="11"/>
-        <v>42</v>
+        <f>K36</f>
+        <v>94</v>
       </c>
       <c r="M36" s="14">
-        <v>457</v>
+        <v>1915</v>
       </c>
       <c r="N36" s="14">
-        <f t="shared" si="12"/>
-        <v>457</v>
+        <f>M36</f>
+        <v>1915</v>
       </c>
       <c r="O36" s="14">
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
       <c r="P36" s="14">
-        <f t="shared" si="13"/>
-        <v>0.52</v>
+        <f>O36</f>
+        <v>0.51</v>
       </c>
       <c r="Q36" s="14">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R36" s="15">
-        <f t="shared" si="14"/>
-        <v>8.1081081081081086E-2</v>
+        <f>Q36/37</f>
+        <v>0.27027027027027029</v>
       </c>
       <c r="S36" s="15">
-        <f t="shared" si="8"/>
-        <v>8.1081081081081086E-2</v>
+        <f>R36</f>
+        <v>0.27027027027027029</v>
       </c>
       <c r="T36" s="15">
         <f>I36/R36</f>
-        <v>5.2721176666666665</v>
+        <v>6.6368491000000001</v>
       </c>
       <c r="U36" s="15">
         <f>T36</f>
-        <v>5.2721176666666665</v>
+        <v>6.6368491000000001</v>
       </c>
       <c r="V36" s="16">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>17</v>
+        <v>243</v>
       </c>
       <c r="C37" s="14">
-        <v>2582580517</v>
+        <v>2619619040</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E37" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>227</v>
+      <c r="E37" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>188</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="H37" s="14">
-        <v>1782609</v>
+        <v>427469</v>
       </c>
       <c r="I37" s="15">
-        <f t="shared" si="9"/>
-        <v>1.7826090000000001</v>
+        <f>H37/1000000</f>
+        <v>0.42746899999999999</v>
       </c>
       <c r="J37" s="15">
-        <f t="shared" si="10"/>
-        <v>1.7826090000000001</v>
+        <f>I37</f>
+        <v>0.42746899999999999</v>
       </c>
       <c r="K37" s="14">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="L37" s="14">
-        <f t="shared" si="11"/>
-        <v>108</v>
+        <f>K37</f>
+        <v>42</v>
       </c>
       <c r="M37" s="14">
-        <v>1884</v>
+        <v>457</v>
       </c>
       <c r="N37" s="14">
-        <f t="shared" si="12"/>
-        <v>1884</v>
+        <f>M37</f>
+        <v>457</v>
       </c>
       <c r="O37" s="14">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="P37" s="14">
-        <f t="shared" si="13"/>
-        <v>0.54</v>
+        <f>O37</f>
+        <v>0.52</v>
       </c>
       <c r="Q37" s="14">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="R37" s="15">
-        <f t="shared" si="14"/>
-        <v>0.35135135135135137</v>
+        <f>Q37/37</f>
+        <v>8.1081081081081086E-2</v>
       </c>
       <c r="S37" s="15">
-        <f t="shared" si="8"/>
-        <v>0.35135135135135137</v>
+        <f>R37</f>
+        <v>8.1081081081081086E-2</v>
       </c>
       <c r="T37" s="15">
-        <f t="shared" si="15"/>
-        <v>5.0735794615384613</v>
+        <f>I37/R37</f>
+        <v>5.2721176666666665</v>
       </c>
       <c r="U37" s="15">
-        <f t="shared" si="16"/>
-        <v>5.0735794615384613</v>
+        <f>T37</f>
+        <v>5.2721176666666665</v>
       </c>
       <c r="V37" s="16">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C38" s="14">
-        <v>2582580520</v>
+        <v>2582580517</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>119</v>
@@ -5156,55 +5156,55 @@
         <v>230</v>
       </c>
       <c r="H38" s="14">
-        <v>1204534</v>
+        <v>1782609</v>
       </c>
       <c r="I38" s="15">
-        <f t="shared" si="9"/>
-        <v>1.204534</v>
+        <f>H38/1000000</f>
+        <v>1.7826090000000001</v>
       </c>
       <c r="J38" s="15">
-        <f t="shared" si="10"/>
-        <v>1.204534</v>
+        <f>I38</f>
+        <v>1.7826090000000001</v>
       </c>
       <c r="K38" s="14">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="L38" s="14">
-        <f t="shared" si="11"/>
-        <v>149</v>
+        <f>K38</f>
+        <v>108</v>
       </c>
       <c r="M38" s="14">
-        <v>1363</v>
+        <v>1884</v>
       </c>
       <c r="N38" s="14">
-        <f t="shared" si="12"/>
-        <v>1363</v>
+        <f>M38</f>
+        <v>1884</v>
       </c>
       <c r="O38" s="14">
-        <v>0.6</v>
+        <v>0.54</v>
       </c>
       <c r="P38" s="14">
-        <f t="shared" si="13"/>
-        <v>0.6</v>
+        <f>O38</f>
+        <v>0.54</v>
       </c>
       <c r="Q38" s="14">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="R38" s="15">
-        <f t="shared" si="14"/>
-        <v>0.83783783783783783</v>
+        <f>Q38/37</f>
+        <v>0.35135135135135137</v>
       </c>
       <c r="S38" s="15">
-        <f t="shared" si="8"/>
-        <v>0.83783783783783783</v>
+        <f>R38</f>
+        <v>0.35135135135135137</v>
       </c>
       <c r="T38" s="15">
-        <f t="shared" si="15"/>
-        <v>1.4376696129032258</v>
+        <f>I38/R38</f>
+        <v>5.0735794615384613</v>
       </c>
       <c r="U38" s="15">
-        <f t="shared" si="16"/>
-        <v>1.4376696129032258</v>
+        <f>T38</f>
+        <v>5.0735794615384613</v>
       </c>
       <c r="V38" s="16">
         <v>6</v>
@@ -5212,13 +5212,13 @@
     </row>
     <row r="39" spans="1:22">
       <c r="A39" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C39" s="14">
-        <v>2582580530</v>
+        <v>2582580520</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>119</v>
@@ -5233,55 +5233,55 @@
         <v>230</v>
       </c>
       <c r="H39" s="14">
-        <v>1498931</v>
+        <v>1204534</v>
       </c>
       <c r="I39" s="15">
-        <f t="shared" si="9"/>
-        <v>1.498931</v>
+        <f>H39/1000000</f>
+        <v>1.204534</v>
       </c>
       <c r="J39" s="15">
-        <f t="shared" si="10"/>
-        <v>1.498931</v>
+        <f>I39</f>
+        <v>1.204534</v>
       </c>
       <c r="K39" s="14">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L39" s="14">
-        <f t="shared" si="11"/>
-        <v>150</v>
+        <f>K39</f>
+        <v>149</v>
       </c>
       <c r="M39" s="14">
-        <v>1632</v>
+        <v>1363</v>
       </c>
       <c r="N39" s="14">
-        <f t="shared" si="12"/>
-        <v>1632</v>
+        <f>M39</f>
+        <v>1363</v>
       </c>
       <c r="O39" s="14">
-        <v>0.51</v>
+        <v>0.6</v>
       </c>
       <c r="P39" s="14">
-        <f t="shared" si="13"/>
-        <v>0.51</v>
+        <f>O39</f>
+        <v>0.6</v>
       </c>
       <c r="Q39" s="14">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="R39" s="15">
-        <f t="shared" si="14"/>
-        <v>0.67567567567567566</v>
+        <f>Q39/37</f>
+        <v>0.83783783783783783</v>
       </c>
       <c r="S39" s="15">
-        <f t="shared" si="8"/>
-        <v>0.67567567567567566</v>
+        <f>R39</f>
+        <v>0.83783783783783783</v>
       </c>
       <c r="T39" s="15">
-        <f t="shared" si="15"/>
-        <v>2.2184178800000001</v>
+        <f>I39/R39</f>
+        <v>1.4376696129032258</v>
       </c>
       <c r="U39" s="15">
-        <f t="shared" si="16"/>
-        <v>2.2184178800000001</v>
+        <f>T39</f>
+        <v>1.4376696129032258</v>
       </c>
       <c r="V39" s="16">
         <v>6</v>
@@ -5289,76 +5289,76 @@
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C40" s="14">
-        <v>2582580539</v>
+        <v>2582580530</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E40" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>123</v>
+      <c r="E40" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>227</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="H40" s="14">
-        <v>1793743</v>
+        <v>1498931</v>
       </c>
       <c r="I40" s="15">
-        <f t="shared" si="9"/>
-        <v>1.7937430000000001</v>
+        <f>H40/1000000</f>
+        <v>1.498931</v>
       </c>
       <c r="J40" s="15">
-        <f t="shared" si="10"/>
-        <v>1.7937430000000001</v>
+        <f>I40</f>
+        <v>1.498931</v>
       </c>
       <c r="K40" s="14">
-        <v>94</v>
+        <v>150</v>
       </c>
       <c r="L40" s="14">
-        <f t="shared" si="11"/>
-        <v>94</v>
+        <f>K40</f>
+        <v>150</v>
       </c>
       <c r="M40" s="14">
-        <v>1915</v>
+        <v>1632</v>
       </c>
       <c r="N40" s="14">
-        <f t="shared" si="12"/>
-        <v>1915</v>
+        <f>M40</f>
+        <v>1632</v>
       </c>
       <c r="O40" s="14">
         <v>0.51</v>
       </c>
       <c r="P40" s="14">
-        <f t="shared" si="13"/>
+        <f>O40</f>
         <v>0.51</v>
       </c>
       <c r="Q40" s="14">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="R40" s="15">
-        <f t="shared" si="14"/>
-        <v>0.27027027027027029</v>
+        <f>Q40/37</f>
+        <v>0.67567567567567566</v>
       </c>
       <c r="S40" s="15">
-        <f t="shared" si="8"/>
-        <v>0.27027027027027029</v>
+        <f>R40</f>
+        <v>0.67567567567567566</v>
       </c>
       <c r="T40" s="15">
-        <f t="shared" si="15"/>
-        <v>6.6368491000000001</v>
+        <f>I40/R40</f>
+        <v>2.2184178800000001</v>
       </c>
       <c r="U40" s="15">
-        <f t="shared" si="16"/>
-        <v>6.6368491000000001</v>
+        <f>T40</f>
+        <v>2.2184178800000001</v>
       </c>
       <c r="V40" s="16">
         <v>6</v>
@@ -5390,51 +5390,51 @@
         <v>2350389</v>
       </c>
       <c r="I41" s="15">
-        <f t="shared" si="9"/>
+        <f>H41/1000000</f>
         <v>2.3503889999999998</v>
       </c>
       <c r="J41" s="15">
-        <f t="shared" si="10"/>
+        <f>I41</f>
         <v>2.3503889999999998</v>
       </c>
       <c r="K41" s="14">
         <v>135</v>
       </c>
       <c r="L41" s="14">
-        <f t="shared" si="11"/>
+        <f>K41</f>
         <v>135</v>
       </c>
       <c r="M41" s="14">
         <v>2379</v>
       </c>
       <c r="N41" s="14">
-        <f t="shared" si="12"/>
+        <f>M41</f>
         <v>2379</v>
       </c>
       <c r="O41" s="14">
         <v>0.67</v>
       </c>
       <c r="P41" s="14">
-        <f t="shared" si="13"/>
+        <f>O41</f>
         <v>0.67</v>
       </c>
       <c r="Q41" s="14">
         <v>32</v>
       </c>
       <c r="R41" s="15">
-        <f t="shared" si="14"/>
+        <f>Q41/37</f>
         <v>0.86486486486486491</v>
       </c>
       <c r="S41" s="15">
-        <f t="shared" si="8"/>
+        <f>R41</f>
         <v>0.86486486486486491</v>
       </c>
       <c r="T41" s="15">
-        <f t="shared" si="15"/>
+        <f>I41/R41</f>
         <v>2.7176372812499996</v>
       </c>
       <c r="U41" s="15">
-        <f t="shared" si="16"/>
+        <f>T41</f>
         <v>2.7176372812499996</v>
       </c>
       <c r="V41" s="16">
@@ -5467,51 +5467,51 @@
         <v>1671027</v>
       </c>
       <c r="I42" s="15">
-        <f t="shared" si="9"/>
+        <f>H42/1000000</f>
         <v>1.671027</v>
       </c>
       <c r="J42" s="15">
-        <f t="shared" si="10"/>
+        <f>I42</f>
         <v>1.671027</v>
       </c>
       <c r="K42" s="14">
         <v>87</v>
       </c>
       <c r="L42" s="14">
-        <f t="shared" si="11"/>
+        <f>K42</f>
         <v>87</v>
       </c>
       <c r="M42" s="14">
         <v>1760</v>
       </c>
       <c r="N42" s="14">
-        <f t="shared" si="12"/>
+        <f>M42</f>
         <v>1760</v>
       </c>
       <c r="O42" s="14">
         <v>0.54</v>
       </c>
       <c r="P42" s="14">
-        <f t="shared" si="13"/>
+        <f>O42</f>
         <v>0.54</v>
       </c>
       <c r="Q42" s="14">
         <v>11</v>
       </c>
       <c r="R42" s="15">
-        <f t="shared" si="14"/>
+        <f>Q42/37</f>
         <v>0.29729729729729731</v>
       </c>
       <c r="S42" s="15">
-        <f t="shared" si="8"/>
+        <f>R42</f>
         <v>0.29729729729729731</v>
       </c>
       <c r="T42" s="15">
-        <f t="shared" si="15"/>
+        <f>I42/R42</f>
         <v>5.6207271818181814</v>
       </c>
       <c r="U42" s="15">
-        <f t="shared" si="16"/>
+        <f>T42</f>
         <v>5.6207271818181814</v>
       </c>
       <c r="V42" s="16">
@@ -5544,51 +5544,51 @@
         <v>1785483</v>
       </c>
       <c r="I43" s="15">
-        <f t="shared" si="9"/>
+        <f>H43/1000000</f>
         <v>1.7854829999999999</v>
       </c>
       <c r="J43" s="15">
-        <f t="shared" si="10"/>
+        <f>I43</f>
         <v>1.7854829999999999</v>
       </c>
       <c r="K43" s="14">
         <v>131</v>
       </c>
       <c r="L43" s="14">
-        <f t="shared" si="11"/>
+        <f>K43</f>
         <v>131</v>
       </c>
       <c r="M43" s="14">
         <v>1934</v>
       </c>
       <c r="N43" s="14">
-        <f t="shared" si="12"/>
+        <f>M43</f>
         <v>1934</v>
       </c>
       <c r="O43" s="14">
         <v>0.52</v>
       </c>
       <c r="P43" s="14">
-        <f t="shared" si="13"/>
+        <f>O43</f>
         <v>0.52</v>
       </c>
       <c r="Q43" s="14">
         <v>30</v>
       </c>
       <c r="R43" s="15">
-        <f t="shared" si="14"/>
+        <f>Q43/37</f>
         <v>0.81081081081081086</v>
       </c>
       <c r="S43" s="15">
-        <f t="shared" si="8"/>
+        <f>R43</f>
         <v>0.81081081081081086</v>
       </c>
       <c r="T43" s="15">
-        <f t="shared" si="15"/>
+        <f>I43/R43</f>
         <v>2.2020956999999997</v>
       </c>
       <c r="U43" s="15">
-        <f t="shared" si="16"/>
+        <f>T43</f>
         <v>2.2020956999999997</v>
       </c>
       <c r="V43" s="16">
@@ -5621,51 +5621,51 @@
         <v>2093635</v>
       </c>
       <c r="I44" s="15">
-        <f t="shared" si="9"/>
+        <f>H44/1000000</f>
         <v>2.0936349999999999</v>
       </c>
       <c r="J44" s="15">
-        <f t="shared" si="10"/>
+        <f>I44</f>
         <v>2.0936349999999999</v>
       </c>
       <c r="K44" s="14">
         <v>166</v>
       </c>
       <c r="L44" s="14">
-        <f t="shared" si="11"/>
+        <f>K44</f>
         <v>166</v>
       </c>
       <c r="M44" s="14">
         <v>2148</v>
       </c>
       <c r="N44" s="14">
-        <f t="shared" si="12"/>
+        <f>M44</f>
         <v>2148</v>
       </c>
       <c r="O44" s="14">
         <v>0.67</v>
       </c>
       <c r="P44" s="14">
-        <f t="shared" si="13"/>
+        <f>O44</f>
         <v>0.67</v>
       </c>
       <c r="Q44" s="14">
         <v>28</v>
       </c>
       <c r="R44" s="15">
-        <f t="shared" si="14"/>
+        <f>Q44/37</f>
         <v>0.7567567567567568</v>
       </c>
       <c r="S44" s="15">
-        <f t="shared" si="8"/>
+        <f>R44</f>
         <v>0.7567567567567568</v>
       </c>
       <c r="T44" s="15">
-        <f t="shared" si="15"/>
+        <f>I44/R44</f>
         <v>2.766589107142857</v>
       </c>
       <c r="U44" s="15">
-        <f t="shared" si="16"/>
+        <f>T44</f>
         <v>2.766589107142857</v>
       </c>
       <c r="V44" s="16">
@@ -5698,51 +5698,51 @@
         <v>764032</v>
       </c>
       <c r="I45" s="15">
-        <f t="shared" si="9"/>
+        <f>H45/1000000</f>
         <v>0.76403200000000004</v>
       </c>
       <c r="J45" s="15">
-        <f t="shared" si="10"/>
+        <f>I45</f>
         <v>0.76403200000000004</v>
       </c>
       <c r="K45" s="14">
         <v>95</v>
       </c>
       <c r="L45" s="14">
-        <f t="shared" si="11"/>
+        <f>K45</f>
         <v>95</v>
       </c>
       <c r="M45" s="14">
         <v>917</v>
       </c>
       <c r="N45" s="14">
-        <f t="shared" si="12"/>
+        <f>M45</f>
         <v>917</v>
       </c>
       <c r="O45" s="14">
         <v>0.55000000000000004</v>
       </c>
       <c r="P45" s="14">
-        <f t="shared" si="13"/>
+        <f>O45</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="Q45" s="14">
         <v>35</v>
       </c>
       <c r="R45" s="15">
-        <f t="shared" si="14"/>
+        <f>Q45/37</f>
         <v>0.94594594594594594</v>
       </c>
       <c r="S45" s="15">
-        <f t="shared" si="8"/>
+        <f>R45</f>
         <v>0.94594594594594594</v>
       </c>
       <c r="T45" s="15">
-        <f t="shared" si="15"/>
+        <f>I45/R45</f>
         <v>0.80769097142857149</v>
       </c>
       <c r="U45" s="15">
-        <f t="shared" si="16"/>
+        <f>T45</f>
         <v>0.80769097142857149</v>
       </c>
       <c r="V45" s="16">
@@ -5775,51 +5775,51 @@
         <v>1010358</v>
       </c>
       <c r="I46" s="15">
-        <f t="shared" si="9"/>
+        <f>H46/1000000</f>
         <v>1.0103580000000001</v>
       </c>
       <c r="J46" s="15">
-        <f t="shared" si="10"/>
+        <f>I46</f>
         <v>1.0103580000000001</v>
       </c>
       <c r="K46" s="14">
         <v>59</v>
       </c>
       <c r="L46" s="14">
-        <f t="shared" si="11"/>
+        <f>K46</f>
         <v>59</v>
       </c>
       <c r="M46" s="14">
         <v>1084</v>
       </c>
       <c r="N46" s="14">
-        <f t="shared" si="12"/>
+        <f>M46</f>
         <v>1084</v>
       </c>
       <c r="O46" s="14">
         <v>0.5</v>
       </c>
       <c r="P46" s="14">
-        <f t="shared" si="13"/>
+        <f>O46</f>
         <v>0.5</v>
       </c>
       <c r="Q46" s="14">
         <v>8</v>
       </c>
       <c r="R46" s="15">
-        <f t="shared" si="14"/>
+        <f>Q46/37</f>
         <v>0.21621621621621623</v>
       </c>
       <c r="S46" s="15">
-        <f t="shared" si="8"/>
+        <f>R46</f>
         <v>0.21621621621621623</v>
       </c>
       <c r="T46" s="15">
-        <f t="shared" si="15"/>
+        <f>I46/R46</f>
         <v>4.67290575</v>
       </c>
       <c r="U46" s="15">
-        <f t="shared" si="16"/>
+        <f>T46</f>
         <v>4.67290575</v>
       </c>
       <c r="V46" s="16">
@@ -5852,51 +5852,51 @@
         <v>1750488</v>
       </c>
       <c r="I47" s="15">
-        <f t="shared" si="9"/>
+        <f>H47/1000000</f>
         <v>1.750488</v>
       </c>
       <c r="J47" s="15">
-        <f t="shared" si="10"/>
+        <f>I47</f>
         <v>1.750488</v>
       </c>
       <c r="K47" s="14">
         <v>204</v>
       </c>
       <c r="L47" s="14">
-        <f t="shared" si="11"/>
+        <f>K47</f>
         <v>204</v>
       </c>
       <c r="M47" s="14">
         <v>1887</v>
       </c>
       <c r="N47" s="14">
-        <f t="shared" si="12"/>
+        <f>M47</f>
         <v>1887</v>
       </c>
       <c r="O47" s="14">
         <v>0.64</v>
       </c>
       <c r="P47" s="14">
-        <f t="shared" si="13"/>
+        <f>O47</f>
         <v>0.64</v>
       </c>
       <c r="Q47" s="14">
         <v>30</v>
       </c>
       <c r="R47" s="15">
-        <f t="shared" si="14"/>
+        <f>Q47/37</f>
         <v>0.81081081081081086</v>
       </c>
       <c r="S47" s="15">
-        <f t="shared" si="8"/>
+        <f>R47</f>
         <v>0.81081081081081086</v>
       </c>
       <c r="T47" s="15">
-        <f t="shared" si="15"/>
+        <f>I47/R47</f>
         <v>2.1589351999999997</v>
       </c>
       <c r="U47" s="15">
-        <f t="shared" si="16"/>
+        <f>T47</f>
         <v>2.1589351999999997</v>
       </c>
       <c r="V47" s="16">
@@ -5929,51 +5929,51 @@
         <v>1267473</v>
       </c>
       <c r="I48" s="15">
-        <f t="shared" si="9"/>
+        <f>H48/1000000</f>
         <v>1.2674730000000001</v>
       </c>
       <c r="J48" s="15">
-        <f t="shared" si="10"/>
+        <f>I48</f>
         <v>1.2674730000000001</v>
       </c>
       <c r="K48" s="14">
         <v>197</v>
       </c>
       <c r="L48" s="14">
-        <f t="shared" si="11"/>
+        <f>K48</f>
         <v>197</v>
       </c>
       <c r="M48" s="14">
         <v>1398</v>
       </c>
       <c r="N48" s="14">
-        <f t="shared" si="12"/>
+        <f>M48</f>
         <v>1398</v>
       </c>
       <c r="O48" s="14">
         <v>0.56000000000000005</v>
       </c>
       <c r="P48" s="14">
-        <f t="shared" si="13"/>
+        <f>O48</f>
         <v>0.56000000000000005</v>
       </c>
       <c r="Q48" s="14">
         <v>33</v>
       </c>
       <c r="R48" s="15">
-        <f t="shared" si="14"/>
+        <f>Q48/37</f>
         <v>0.89189189189189189</v>
       </c>
       <c r="S48" s="15">
-        <f t="shared" si="8"/>
+        <f>R48</f>
         <v>0.89189189189189189</v>
       </c>
       <c r="T48" s="15">
-        <f t="shared" si="15"/>
+        <f>I48/R48</f>
         <v>1.4211060909090909</v>
       </c>
       <c r="U48" s="15">
-        <f t="shared" si="16"/>
+        <f>T48</f>
         <v>1.4211060909090909</v>
       </c>
       <c r="V48" s="16">
@@ -6006,51 +6006,51 @@
         <v>1149636</v>
       </c>
       <c r="I49" s="15">
-        <f t="shared" si="9"/>
+        <f>H49/1000000</f>
         <v>1.1496360000000001</v>
       </c>
       <c r="J49" s="15">
-        <f t="shared" si="10"/>
+        <f>I49</f>
         <v>1.1496360000000001</v>
       </c>
       <c r="K49" s="14">
         <v>85</v>
       </c>
       <c r="L49" s="14">
-        <f t="shared" si="11"/>
+        <f>K49</f>
         <v>85</v>
       </c>
       <c r="M49" s="14">
         <v>1251</v>
       </c>
       <c r="N49" s="14">
-        <f t="shared" si="12"/>
+        <f>M49</f>
         <v>1251</v>
       </c>
       <c r="O49" s="14">
         <v>0.5</v>
       </c>
       <c r="P49" s="14">
-        <f t="shared" si="13"/>
+        <f>O49</f>
         <v>0.5</v>
       </c>
       <c r="Q49" s="14">
         <v>5</v>
       </c>
       <c r="R49" s="15">
-        <f t="shared" si="14"/>
+        <f>Q49/37</f>
         <v>0.13513513513513514</v>
       </c>
       <c r="S49" s="15">
-        <f t="shared" si="8"/>
+        <f>R49</f>
         <v>0.13513513513513514</v>
       </c>
       <c r="T49" s="15">
-        <f t="shared" si="15"/>
+        <f>I49/R49</f>
         <v>8.5073064000000009</v>
       </c>
       <c r="U49" s="15">
-        <f t="shared" si="16"/>
+        <f>T49</f>
         <v>8.5073064000000009</v>
       </c>
       <c r="V49" s="16">
@@ -6083,51 +6083,51 @@
         <v>1170081</v>
       </c>
       <c r="I50" s="15">
-        <f t="shared" si="9"/>
+        <f>H50/1000000</f>
         <v>1.1700809999999999</v>
       </c>
       <c r="J50" s="15">
-        <f t="shared" si="10"/>
+        <f>I50</f>
         <v>1.1700809999999999</v>
       </c>
       <c r="K50" s="14">
         <v>108</v>
       </c>
       <c r="L50" s="14">
-        <f t="shared" si="11"/>
+        <f>K50</f>
         <v>108</v>
       </c>
       <c r="M50" s="14">
         <v>1319</v>
       </c>
       <c r="N50" s="14">
-        <f t="shared" si="12"/>
+        <f>M50</f>
         <v>1319</v>
       </c>
       <c r="O50" s="14">
         <v>0.55000000000000004</v>
       </c>
       <c r="P50" s="14">
-        <f t="shared" si="13"/>
+        <f>O50</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="Q50" s="14">
         <v>28</v>
       </c>
       <c r="R50" s="15">
-        <f t="shared" si="14"/>
+        <f>Q50/37</f>
         <v>0.7567567567567568</v>
       </c>
       <c r="S50" s="15">
-        <f t="shared" si="8"/>
+        <f>R50</f>
         <v>0.7567567567567568</v>
       </c>
       <c r="T50" s="15">
-        <f t="shared" si="15"/>
+        <f>I50/R50</f>
         <v>1.5461784642857141</v>
       </c>
       <c r="U50" s="15">
-        <f t="shared" si="16"/>
+        <f>T50</f>
         <v>1.5461784642857141</v>
       </c>
       <c r="V50" s="16">
@@ -6160,51 +6160,51 @@
         <v>1315659</v>
       </c>
       <c r="I51" s="15">
-        <f t="shared" si="9"/>
+        <f>H51/1000000</f>
         <v>1.3156589999999999</v>
       </c>
       <c r="J51" s="15">
-        <f t="shared" si="10"/>
+        <f>I51</f>
         <v>1.3156589999999999</v>
       </c>
       <c r="K51" s="14">
         <v>42</v>
       </c>
       <c r="L51" s="14">
-        <f t="shared" si="11"/>
+        <f>K51</f>
         <v>42</v>
       </c>
       <c r="M51" s="14">
         <v>1392</v>
       </c>
       <c r="N51" s="14">
-        <f t="shared" si="12"/>
+        <f>M51</f>
         <v>1392</v>
       </c>
       <c r="O51" s="14">
         <v>0.56000000000000005</v>
       </c>
       <c r="P51" s="14">
-        <f t="shared" si="13"/>
+        <f>O51</f>
         <v>0.56000000000000005</v>
       </c>
       <c r="Q51" s="14">
         <v>37</v>
       </c>
       <c r="R51" s="15">
-        <f t="shared" si="14"/>
+        <f>Q51/37</f>
         <v>1</v>
       </c>
       <c r="S51" s="15">
-        <f t="shared" si="8"/>
+        <f>R51</f>
         <v>1</v>
       </c>
       <c r="T51" s="15">
-        <f t="shared" si="15"/>
+        <f>I51/R51</f>
         <v>1.3156589999999999</v>
       </c>
       <c r="U51" s="15">
-        <f t="shared" si="16"/>
+        <f>T51</f>
         <v>1.3156589999999999</v>
       </c>
       <c r="V51" s="16">
@@ -6237,51 +6237,51 @@
         <v>795830</v>
       </c>
       <c r="I52" s="15">
-        <f t="shared" si="9"/>
+        <f>H52/1000000</f>
         <v>0.79583000000000004</v>
       </c>
       <c r="J52" s="15">
-        <f t="shared" si="10"/>
+        <f>I52</f>
         <v>0.79583000000000004</v>
       </c>
       <c r="K52" s="14">
         <v>188</v>
       </c>
       <c r="L52" s="14">
-        <f t="shared" si="11"/>
+        <f>K52</f>
         <v>188</v>
       </c>
       <c r="M52" s="14">
         <v>962</v>
       </c>
       <c r="N52" s="14">
-        <f t="shared" si="12"/>
+        <f>M52</f>
         <v>962</v>
       </c>
       <c r="O52" s="14">
         <v>0.64</v>
       </c>
       <c r="P52" s="14">
-        <f t="shared" si="13"/>
+        <f>O52</f>
         <v>0.64</v>
       </c>
       <c r="Q52" s="14">
         <v>17</v>
       </c>
       <c r="R52" s="15">
-        <f t="shared" si="14"/>
+        <f>Q52/37</f>
         <v>0.45945945945945948</v>
       </c>
       <c r="S52" s="15">
-        <f t="shared" si="8"/>
+        <f>R52</f>
         <v>0.45945945945945948</v>
       </c>
       <c r="T52" s="15">
-        <f t="shared" si="15"/>
+        <f>I52/R52</f>
         <v>1.732100588235294</v>
       </c>
       <c r="U52" s="15">
-        <f t="shared" si="16"/>
+        <f>T52</f>
         <v>1.732100588235294</v>
       </c>
       <c r="V52" s="16">
@@ -6314,51 +6314,51 @@
         <v>985902</v>
       </c>
       <c r="I53" s="15">
-        <f t="shared" si="9"/>
+        <f>H53/1000000</f>
         <v>0.98590199999999995</v>
       </c>
       <c r="J53" s="15">
-        <f t="shared" si="10"/>
+        <f>I53</f>
         <v>0.98590199999999995</v>
       </c>
       <c r="K53" s="14">
         <v>27</v>
       </c>
       <c r="L53" s="14">
-        <f t="shared" si="11"/>
+        <f>K53</f>
         <v>27</v>
       </c>
       <c r="M53" s="14">
         <v>1007</v>
       </c>
       <c r="N53" s="14">
-        <f t="shared" si="12"/>
+        <f>M53</f>
         <v>1007</v>
       </c>
       <c r="O53" s="14">
         <v>0.49</v>
       </c>
       <c r="P53" s="14">
-        <f t="shared" si="13"/>
+        <f>O53</f>
         <v>0.49</v>
       </c>
       <c r="Q53" s="14">
         <v>31</v>
       </c>
       <c r="R53" s="15">
-        <f t="shared" si="14"/>
+        <f>Q53/37</f>
         <v>0.83783783783783783</v>
       </c>
       <c r="S53" s="15">
-        <f t="shared" si="8"/>
+        <f>R53</f>
         <v>0.83783783783783783</v>
       </c>
       <c r="T53" s="15">
-        <f t="shared" si="15"/>
+        <f>I53/R53</f>
         <v>1.1767217419354838</v>
       </c>
       <c r="U53" s="15">
-        <f t="shared" si="16"/>
+        <f>T53</f>
         <v>1.1767217419354838</v>
       </c>
       <c r="V53" s="16">
@@ -6391,51 +6391,51 @@
         <v>1050638</v>
       </c>
       <c r="I54" s="15">
-        <f t="shared" si="9"/>
+        <f>H54/1000000</f>
         <v>1.050638</v>
       </c>
       <c r="J54" s="15">
-        <f t="shared" si="10"/>
+        <f>I54</f>
         <v>1.050638</v>
       </c>
       <c r="K54" s="14">
         <v>36</v>
       </c>
       <c r="L54" s="14">
-        <f t="shared" si="11"/>
+        <f>K54</f>
         <v>36</v>
       </c>
       <c r="M54" s="14">
         <v>1050</v>
       </c>
       <c r="N54" s="14">
-        <f t="shared" si="12"/>
+        <f>M54</f>
         <v>1050</v>
       </c>
       <c r="O54" s="14">
         <v>0.46</v>
       </c>
       <c r="P54" s="14">
-        <f t="shared" si="13"/>
+        <f>O54</f>
         <v>0.46</v>
       </c>
       <c r="Q54" s="14">
         <v>8</v>
       </c>
       <c r="R54" s="15">
-        <f t="shared" si="14"/>
+        <f>Q54/37</f>
         <v>0.21621621621621623</v>
       </c>
       <c r="S54" s="15">
-        <f t="shared" si="8"/>
+        <f>R54</f>
         <v>0.21621621621621623</v>
       </c>
       <c r="T54" s="15">
-        <f t="shared" si="15"/>
+        <f>I54/R54</f>
         <v>4.8592007499999994</v>
       </c>
       <c r="U54" s="15">
-        <f t="shared" si="16"/>
+        <f>T54</f>
         <v>4.8592007499999994</v>
       </c>
       <c r="V54" s="16">
@@ -6468,51 +6468,51 @@
         <v>1072419</v>
       </c>
       <c r="I55" s="15">
-        <f t="shared" si="9"/>
+        <f>H55/1000000</f>
         <v>1.072419</v>
       </c>
       <c r="J55" s="15">
-        <f t="shared" si="10"/>
+        <f>I55</f>
         <v>1.072419</v>
       </c>
       <c r="K55" s="14">
         <v>109</v>
       </c>
       <c r="L55" s="14">
-        <f t="shared" si="11"/>
+        <f>K55</f>
         <v>109</v>
       </c>
       <c r="M55" s="14">
         <v>1136</v>
       </c>
       <c r="N55" s="14">
-        <f t="shared" si="12"/>
+        <f>M55</f>
         <v>1136</v>
       </c>
       <c r="O55" s="14">
         <v>0.44</v>
       </c>
       <c r="P55" s="14">
-        <f t="shared" si="13"/>
+        <f>O55</f>
         <v>0.44</v>
       </c>
       <c r="Q55" s="14">
         <v>9</v>
       </c>
       <c r="R55" s="15">
-        <f t="shared" si="14"/>
+        <f>Q55/37</f>
         <v>0.24324324324324326</v>
       </c>
       <c r="S55" s="15">
-        <f t="shared" si="8"/>
+        <f>R55</f>
         <v>0.24324324324324326</v>
       </c>
       <c r="T55" s="15">
-        <f t="shared" si="15"/>
+        <f>I55/R55</f>
         <v>4.4088336666666663</v>
       </c>
       <c r="U55" s="15">
-        <f t="shared" si="16"/>
+        <f>T55</f>
         <v>4.4088336666666663</v>
       </c>
       <c r="V55" s="16">
@@ -6545,51 +6545,51 @@
         <v>2533346</v>
       </c>
       <c r="I56" s="15">
-        <f t="shared" si="9"/>
+        <f>H56/1000000</f>
         <v>2.5333459999999999</v>
       </c>
       <c r="J56" s="15">
-        <f t="shared" si="10"/>
+        <f>I56</f>
         <v>2.5333459999999999</v>
       </c>
       <c r="K56" s="14">
         <v>444</v>
       </c>
       <c r="L56" s="14">
-        <f t="shared" si="11"/>
+        <f>K56</f>
         <v>444</v>
       </c>
       <c r="M56" s="14">
         <v>2717</v>
       </c>
       <c r="N56" s="14">
-        <f t="shared" si="12"/>
+        <f>M56</f>
         <v>2717</v>
       </c>
       <c r="O56" s="14">
         <v>0.69</v>
       </c>
       <c r="P56" s="14">
-        <f t="shared" si="13"/>
+        <f>O56</f>
         <v>0.69</v>
       </c>
       <c r="Q56" s="14">
         <v>29</v>
       </c>
       <c r="R56" s="15">
-        <f t="shared" si="14"/>
+        <f>Q56/37</f>
         <v>0.78378378378378377</v>
       </c>
       <c r="S56" s="15">
-        <f t="shared" si="8"/>
+        <f>R56</f>
         <v>0.78378378378378377</v>
       </c>
       <c r="T56" s="15">
-        <f t="shared" si="15"/>
+        <f>I56/R56</f>
         <v>3.232200068965517</v>
       </c>
       <c r="U56" s="15">
-        <f t="shared" si="16"/>
+        <f>T56</f>
         <v>3.232200068965517</v>
       </c>
       <c r="V56" s="16">
@@ -6669,7 +6669,7 @@
         <v>0</v>
       </c>
       <c r="S59" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="S3:S65" si="0">R59</f>
         <v>0</v>
       </c>
       <c r="T59" s="15" t="e">
@@ -6746,7 +6746,7 @@
         <v>0</v>
       </c>
       <c r="S60" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T60" s="15" t="e">
@@ -6834,7 +6834,7 @@
         <v>0.24324324324324326</v>
       </c>
       <c r="S63" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>0.24324324324324326</v>
       </c>
       <c r="T63" s="15">
@@ -6911,7 +6911,7 @@
         <v>0.1891891891891892</v>
       </c>
       <c r="S64" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>0.1891891891891892</v>
       </c>
       <c r="T64" s="15">
@@ -6980,7 +6980,7 @@
         <v>0.32432432432432434</v>
       </c>
       <c r="S65" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>0.32432432432432434</v>
       </c>
       <c r="T65" s="15">
@@ -7145,28 +7145,28 @@
         <v>0.97</v>
       </c>
       <c r="J69" s="15">
-        <f t="shared" ref="J69:J78" si="17">I69</f>
+        <f t="shared" ref="J69:J78" si="1">I69</f>
         <v>0.97</v>
       </c>
       <c r="K69" s="13">
         <v>37</v>
       </c>
       <c r="L69" s="14">
-        <f t="shared" ref="L69:L78" si="18">K69</f>
+        <f t="shared" ref="L69:L78" si="2">K69</f>
         <v>37</v>
       </c>
       <c r="M69" s="13">
         <v>965</v>
       </c>
       <c r="N69" s="14">
-        <f t="shared" ref="N69:N78" si="19">M69</f>
+        <f t="shared" ref="N69:N78" si="3">M69</f>
         <v>965</v>
       </c>
       <c r="O69" s="17">
         <v>0.56999999999999995</v>
       </c>
       <c r="P69" s="14">
-        <f t="shared" ref="P69:P78" si="20">O69</f>
+        <f t="shared" ref="P69:P78" si="4">O69</f>
         <v>0.56999999999999995</v>
       </c>
       <c r="Q69" s="13">
@@ -7183,7 +7183,7 @@
         <v>1.24</v>
       </c>
       <c r="U69" s="15">
-        <f t="shared" ref="U69:U78" si="21">T69</f>
+        <f t="shared" ref="U69:U78" si="5">T69</f>
         <v>1.24</v>
       </c>
       <c r="V69" s="18">
@@ -7217,28 +7217,28 @@
         <v>1.24</v>
       </c>
       <c r="J70" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>1.24</v>
       </c>
       <c r="K70" s="13">
         <v>10</v>
       </c>
       <c r="L70" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="M70" s="13">
         <v>1259</v>
       </c>
       <c r="N70" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>1259</v>
       </c>
       <c r="O70" s="17">
         <v>0.44</v>
       </c>
       <c r="P70" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="4"/>
         <v>0.44</v>
       </c>
       <c r="Q70" s="13">
@@ -7255,7 +7255,7 @@
         <v>1.28</v>
       </c>
       <c r="U70" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="5"/>
         <v>1.28</v>
       </c>
       <c r="V70" s="18">
@@ -7286,51 +7286,51 @@
         <v>523140</v>
       </c>
       <c r="I71" s="15">
-        <f t="shared" ref="I71:I78" si="22">H71/1000000</f>
+        <f t="shared" ref="I71:I78" si="6">H71/1000000</f>
         <v>0.52314000000000005</v>
       </c>
       <c r="J71" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>0.52314000000000005</v>
       </c>
       <c r="K71" s="14">
         <v>31</v>
       </c>
       <c r="L71" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="M71" s="14">
         <v>551</v>
       </c>
       <c r="N71" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>551</v>
       </c>
       <c r="O71" s="15">
         <v>0.42059999999999997</v>
       </c>
       <c r="P71" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="4"/>
         <v>0.42059999999999997</v>
       </c>
       <c r="Q71" s="14">
         <v>3</v>
       </c>
       <c r="R71" s="15">
-        <f t="shared" ref="R71:R78" si="23">Q71/37</f>
+        <f t="shared" ref="R71:R78" si="7">Q71/37</f>
         <v>8.1081081081081086E-2</v>
       </c>
       <c r="S71" s="15">
-        <f t="shared" ref="S71:S78" si="24">R71</f>
+        <f t="shared" ref="S71:S78" si="8">R71</f>
         <v>8.1081081081081086E-2</v>
       </c>
       <c r="T71" s="15">
-        <f t="shared" ref="T71:T78" si="25">I71/R71</f>
+        <f t="shared" ref="T71:T78" si="9">I71/R71</f>
         <v>6.4520600000000004</v>
       </c>
       <c r="U71" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="5"/>
         <v>6.4520600000000004</v>
       </c>
       <c r="V71" s="16">
@@ -7361,51 +7361,51 @@
         <v>974886</v>
       </c>
       <c r="I72" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="6"/>
         <v>0.97488600000000003</v>
       </c>
       <c r="J72" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>0.97488600000000003</v>
       </c>
       <c r="K72" s="14">
         <v>66</v>
       </c>
       <c r="L72" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="M72" s="14">
         <v>1004</v>
       </c>
       <c r="N72" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>1004</v>
       </c>
       <c r="O72" s="15">
         <v>0.4042</v>
       </c>
       <c r="P72" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="4"/>
         <v>0.4042</v>
       </c>
       <c r="Q72" s="14">
         <v>6</v>
       </c>
       <c r="R72" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="7"/>
         <v>0.16216216216216217</v>
       </c>
       <c r="S72" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="8"/>
         <v>0.16216216216216217</v>
       </c>
       <c r="T72" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="9"/>
         <v>6.0117969999999996</v>
       </c>
       <c r="U72" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="5"/>
         <v>6.0117969999999996</v>
       </c>
       <c r="V72" s="16">
@@ -7436,51 +7436,51 @@
         <v>856463</v>
       </c>
       <c r="I73" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="6"/>
         <v>0.85646299999999997</v>
       </c>
       <c r="J73" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>0.85646299999999997</v>
       </c>
       <c r="K73" s="14">
         <v>36</v>
       </c>
       <c r="L73" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="M73" s="14">
         <v>873</v>
       </c>
       <c r="N73" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>873</v>
       </c>
       <c r="O73" s="15">
         <v>0.61639999999999995</v>
       </c>
       <c r="P73" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="4"/>
         <v>0.61639999999999995</v>
       </c>
       <c r="Q73" s="14">
         <v>29</v>
       </c>
       <c r="R73" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="7"/>
         <v>0.78378378378378377</v>
       </c>
       <c r="S73" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="8"/>
         <v>0.78378378378378377</v>
       </c>
       <c r="T73" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="9"/>
         <v>1.0927286551724138</v>
       </c>
       <c r="U73" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="5"/>
         <v>1.0927286551724138</v>
       </c>
       <c r="V73" s="16">
@@ -7511,51 +7511,51 @@
         <v>1083653</v>
       </c>
       <c r="I74" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="6"/>
         <v>1.083653</v>
       </c>
       <c r="J74" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>1.083653</v>
       </c>
       <c r="K74" s="14">
         <v>15</v>
       </c>
       <c r="L74" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M74" s="14">
         <v>1114</v>
       </c>
       <c r="N74" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>1114</v>
       </c>
       <c r="O74" s="15">
         <v>0.59279999999999999</v>
       </c>
       <c r="P74" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="4"/>
         <v>0.59279999999999999</v>
       </c>
       <c r="Q74" s="14">
         <v>33</v>
       </c>
       <c r="R74" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="7"/>
         <v>0.89189189189189189</v>
       </c>
       <c r="S74" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="8"/>
         <v>0.89189189189189189</v>
       </c>
       <c r="T74" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="9"/>
         <v>1.2150048787878787</v>
       </c>
       <c r="U74" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="5"/>
         <v>1.2150048787878787</v>
       </c>
       <c r="V74" s="16">
@@ -7586,49 +7586,49 @@
         <v>979038</v>
       </c>
       <c r="I75" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="6"/>
         <v>0.97903799999999996</v>
       </c>
       <c r="J75" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>0.97903799999999996</v>
       </c>
       <c r="K75" s="14">
         <v>95</v>
       </c>
       <c r="L75" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="M75" s="14">
         <v>1171</v>
       </c>
       <c r="N75" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>1171</v>
       </c>
       <c r="O75" s="14"/>
       <c r="P75" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q75" s="14">
         <v>24</v>
       </c>
       <c r="R75" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="7"/>
         <v>0.64864864864864868</v>
       </c>
       <c r="S75" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="8"/>
         <v>0.64864864864864868</v>
       </c>
       <c r="T75" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="9"/>
         <v>1.5093502499999998</v>
       </c>
       <c r="U75" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="5"/>
         <v>1.5093502499999998</v>
       </c>
       <c r="V75" s="16">
@@ -7659,49 +7659,49 @@
         <v>1340901</v>
       </c>
       <c r="I76" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="6"/>
         <v>1.3409009999999999</v>
       </c>
       <c r="J76" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>1.3409009999999999</v>
       </c>
       <c r="K76" s="14">
         <v>384</v>
       </c>
       <c r="L76" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>384</v>
       </c>
       <c r="M76" s="14">
         <v>1849</v>
       </c>
       <c r="N76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>1849</v>
       </c>
       <c r="O76" s="14"/>
       <c r="P76" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q76" s="14">
         <v>23</v>
       </c>
       <c r="R76" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="7"/>
         <v>0.6216216216216216</v>
       </c>
       <c r="S76" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="8"/>
         <v>0.6216216216216216</v>
       </c>
       <c r="T76" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="9"/>
         <v>2.157101608695652</v>
       </c>
       <c r="U76" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="5"/>
         <v>2.157101608695652</v>
       </c>
       <c r="V76" s="16">
@@ -7734,51 +7734,51 @@
         <v>2582396</v>
       </c>
       <c r="I77" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="6"/>
         <v>2.5823960000000001</v>
       </c>
       <c r="J77" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>2.5823960000000001</v>
       </c>
       <c r="K77" s="14">
         <v>13</v>
       </c>
       <c r="L77" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="M77" s="14">
         <v>2415</v>
       </c>
       <c r="N77" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>2415</v>
       </c>
       <c r="O77" s="14">
         <v>0.61</v>
       </c>
       <c r="P77" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="4"/>
         <v>0.61</v>
       </c>
       <c r="Q77" s="14">
         <v>37</v>
       </c>
       <c r="R77" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S77" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T77" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="9"/>
         <v>2.5823960000000001</v>
       </c>
       <c r="U77" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="5"/>
         <v>2.5823960000000001</v>
       </c>
       <c r="V77" s="16">
@@ -7811,51 +7811,51 @@
         <v>1964596</v>
       </c>
       <c r="I78" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="6"/>
         <v>1.964596</v>
       </c>
       <c r="J78" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>1.964596</v>
       </c>
       <c r="K78" s="14">
         <v>105</v>
       </c>
       <c r="L78" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="M78" s="14">
         <v>2108</v>
       </c>
       <c r="N78" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>2108</v>
       </c>
       <c r="O78" s="14">
         <v>0.49</v>
       </c>
       <c r="P78" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="4"/>
         <v>0.49</v>
       </c>
       <c r="Q78" s="14">
         <v>13</v>
       </c>
       <c r="R78" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="7"/>
         <v>0.35135135135135137</v>
       </c>
       <c r="S78" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="8"/>
         <v>0.35135135135135137</v>
       </c>
       <c r="T78" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="9"/>
         <v>5.5915424615384612</v>
       </c>
       <c r="U78" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="5"/>
         <v>5.5915424615384612</v>
       </c>
       <c r="V78" s="16">
@@ -7863,8 +7863,11 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:U60">
-    <sortCondition ref="A71"/>
+  <sortState ref="A2:V56">
+    <sortCondition ref="D2:D56"/>
+    <sortCondition ref="E2:E56"/>
+    <sortCondition ref="F2:F56"/>
+    <sortCondition ref="A2:A56"/>
   </sortState>
   <conditionalFormatting sqref="P59:P60 P2:P47 P63:P67">
     <cfRule type="dataBar" priority="14">

</xml_diff>